<commit_message>
Update 9350 info (no CSF required anymore)
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -146,205 +146,205 @@
     <t>C2B return</t>
   </si>
   <si>
+    <t>Retur pakke i postkassen</t>
+  </si>
+  <si>
+    <t>9650</t>
+  </si>
+  <si>
+    <t>Retur pakke fra bedrift</t>
+  </si>
+  <si>
+    <t>9000</t>
+  </si>
+  <si>
+    <t>B2B return</t>
+  </si>
+  <si>
+    <t>Returekspress</t>
+  </si>
+  <si>
+    <t>9600</t>
+  </si>
+  <si>
+    <t>Parcel Sweden, Denmark, Finland &amp; Parcel Norway cross-border</t>
+  </si>
+  <si>
+    <t>PickUp Parcel</t>
+  </si>
+  <si>
+    <t>0340</t>
+  </si>
+  <si>
+    <t>PICKUP_PARCEL</t>
+  </si>
+  <si>
+    <t>SE, DK</t>
+  </si>
+  <si>
+    <t>NO, SE, DK, FI</t>
+  </si>
+  <si>
+    <t>ALL COUNTRIES EXCEPT RUSSIA &amp; BELARUS</t>
+  </si>
+  <si>
+    <t>PickUp Parcel Bulk</t>
+  </si>
+  <si>
+    <t>0342</t>
+  </si>
+  <si>
+    <t>PICKUP_PARCEL_BULK</t>
+  </si>
+  <si>
+    <t>Bulk setup</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>NO, SE, DK, FI, DE, EE, FO, GB, IS, NL</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>Home Delivery Parcel</t>
+  </si>
+  <si>
+    <t>0349</t>
+  </si>
+  <si>
+    <t>HOME_DELIVERY_PARCEL</t>
+  </si>
+  <si>
+    <t>NO, SE, DK</t>
+  </si>
+  <si>
+    <t>Business Parcel</t>
+  </si>
+  <si>
+    <t>0330</t>
+  </si>
+  <si>
+    <t>BUSINESS_PARCEL</t>
+  </si>
+  <si>
+    <t>SE, DK, FI</t>
+  </si>
+  <si>
+    <t>Business Parcel Bulk</t>
+  </si>
+  <si>
+    <t>0332</t>
+  </si>
+  <si>
+    <t>BUSINESS_PARCEL_BULK</t>
+  </si>
+  <si>
+    <t>SE, FI</t>
+  </si>
+  <si>
+    <t>Express Nordic 09:00</t>
+  </si>
+  <si>
+    <t>0335</t>
+  </si>
+  <si>
+    <t>EXPRESS_NORDIC_0900</t>
+  </si>
+  <si>
+    <t>Express Nordic 09:00 Bulk</t>
+  </si>
+  <si>
+    <t>0334</t>
+  </si>
+  <si>
+    <t>EXPRESS_NORDIC_0900_BULK</t>
+  </si>
+  <si>
+    <t>NO, SE</t>
+  </si>
+  <si>
+    <t>Business Pallet</t>
+  </si>
+  <si>
+    <t>0336</t>
+  </si>
+  <si>
+    <t>BUSINESS_PALLET</t>
+  </si>
+  <si>
+    <t>NO, SE, DK, FI, AT, AX, BE, CH, CZ, DE, EE, ES, FO, FR, GB, GL, GR, HU, IE, IS, IT, LT, LU, LV, NL, PL, PT, SI, SK</t>
+  </si>
+  <si>
+    <t>Business Pallet (1/2 pallet)</t>
+  </si>
+  <si>
+    <t>BUSINESS_HALFPALLET</t>
+  </si>
+  <si>
+    <t>Business Pallet (1/4 pallet)</t>
+  </si>
+  <si>
+    <t>BUSINESS_QUARTERPALLET</t>
+  </si>
+  <si>
+    <t>PickUp Parcel Return</t>
+  </si>
+  <si>
+    <t>0341</t>
+  </si>
+  <si>
+    <t>PICKUP_PARCEL_RETURN</t>
+  </si>
+  <si>
+    <t>Return setup</t>
+  </si>
+  <si>
+    <t>PickUp Parcel Return Bulk</t>
+  </si>
+  <si>
+    <t>0343</t>
+  </si>
+  <si>
+    <t>PICKUP_PARCEL_RETURN_BULK</t>
+  </si>
+  <si>
+    <t>Business Parcel Return</t>
+  </si>
+  <si>
+    <t>0331</t>
+  </si>
+  <si>
+    <t>BUSINESS_PARCEL_RETURN</t>
+  </si>
+  <si>
+    <t>Business Parcel Return Bulk</t>
+  </si>
+  <si>
+    <t>0333</t>
+  </si>
+  <si>
+    <t>BUSINESS_PARCEL_RETURN_BULK</t>
+  </si>
+  <si>
+    <t>Cargo Norway domestic</t>
+  </si>
+  <si>
+    <t>Stykkgods til bedrift</t>
+  </si>
+  <si>
+    <t>5100</t>
+  </si>
+  <si>
+    <t>Pall til bedrift</t>
+  </si>
+  <si>
+    <t>5400</t>
+  </si>
+  <si>
     <t>Customer setup</t>
-  </si>
-  <si>
-    <t>Retur pakke i postkassen</t>
-  </si>
-  <si>
-    <t>9650</t>
-  </si>
-  <si>
-    <t>Retur pakke fra bedrift</t>
-  </si>
-  <si>
-    <t>9000</t>
-  </si>
-  <si>
-    <t>B2B return</t>
-  </si>
-  <si>
-    <t>Returekspress</t>
-  </si>
-  <si>
-    <t>9600</t>
-  </si>
-  <si>
-    <t>Parcel Sweden, Denmark, Finland &amp; Parcel Norway cross-border</t>
-  </si>
-  <si>
-    <t>PickUp Parcel</t>
-  </si>
-  <si>
-    <t>0340</t>
-  </si>
-  <si>
-    <t>PICKUP_PARCEL</t>
-  </si>
-  <si>
-    <t>SE, DK</t>
-  </si>
-  <si>
-    <t>NO, SE, DK, FI</t>
-  </si>
-  <si>
-    <t>ALL COUNTRIES EXCEPT RUSSIA &amp; BELARUS</t>
-  </si>
-  <si>
-    <t>PickUp Parcel Bulk</t>
-  </si>
-  <si>
-    <t>0342</t>
-  </si>
-  <si>
-    <t>PICKUP_PARCEL_BULK</t>
-  </si>
-  <si>
-    <t>Bulk setup</t>
-  </si>
-  <si>
-    <t>ALL</t>
-  </si>
-  <si>
-    <t>NO, SE, DK, FI, DE, EE, FO, GB, IS, NL</t>
-  </si>
-  <si>
-    <t>SE</t>
-  </si>
-  <si>
-    <t>Home Delivery Parcel</t>
-  </si>
-  <si>
-    <t>0349</t>
-  </si>
-  <si>
-    <t>HOME_DELIVERY_PARCEL</t>
-  </si>
-  <si>
-    <t>NO, SE, DK</t>
-  </si>
-  <si>
-    <t>Business Parcel</t>
-  </si>
-  <si>
-    <t>0330</t>
-  </si>
-  <si>
-    <t>BUSINESS_PARCEL</t>
-  </si>
-  <si>
-    <t>SE, DK, FI</t>
-  </si>
-  <si>
-    <t>Business Parcel Bulk</t>
-  </si>
-  <si>
-    <t>0332</t>
-  </si>
-  <si>
-    <t>BUSINESS_PARCEL_BULK</t>
-  </si>
-  <si>
-    <t>SE, FI</t>
-  </si>
-  <si>
-    <t>Express Nordic 09:00</t>
-  </si>
-  <si>
-    <t>0335</t>
-  </si>
-  <si>
-    <t>EXPRESS_NORDIC_0900</t>
-  </si>
-  <si>
-    <t>Express Nordic 09:00 Bulk</t>
-  </si>
-  <si>
-    <t>0334</t>
-  </si>
-  <si>
-    <t>EXPRESS_NORDIC_0900_BULK</t>
-  </si>
-  <si>
-    <t>NO, SE</t>
-  </si>
-  <si>
-    <t>Business Pallet</t>
-  </si>
-  <si>
-    <t>0336</t>
-  </si>
-  <si>
-    <t>BUSINESS_PALLET</t>
-  </si>
-  <si>
-    <t>NO, SE, DK, FI, AT, AX, BE, CH, CZ, DE, EE, ES, FO, FR, GB, GL, GR, HU, IE, IS, IT, LT, LU, LV, NL, PL, PT, SI, SK</t>
-  </si>
-  <si>
-    <t>Business Pallet (1/2 pallet)</t>
-  </si>
-  <si>
-    <t>BUSINESS_HALFPALLET</t>
-  </si>
-  <si>
-    <t>Business Pallet (1/4 pallet)</t>
-  </si>
-  <si>
-    <t>BUSINESS_QUARTERPALLET</t>
-  </si>
-  <si>
-    <t>PickUp Parcel Return</t>
-  </si>
-  <si>
-    <t>0341</t>
-  </si>
-  <si>
-    <t>PICKUP_PARCEL_RETURN</t>
-  </si>
-  <si>
-    <t>Return setup</t>
-  </si>
-  <si>
-    <t>PickUp Parcel Return Bulk</t>
-  </si>
-  <si>
-    <t>0343</t>
-  </si>
-  <si>
-    <t>PICKUP_PARCEL_RETURN_BULK</t>
-  </si>
-  <si>
-    <t>Business Parcel Return</t>
-  </si>
-  <si>
-    <t>0331</t>
-  </si>
-  <si>
-    <t>BUSINESS_PARCEL_RETURN</t>
-  </si>
-  <si>
-    <t>Business Parcel Return Bulk</t>
-  </si>
-  <si>
-    <t>0333</t>
-  </si>
-  <si>
-    <t>BUSINESS_PARCEL_RETURN_BULK</t>
-  </si>
-  <si>
-    <t>Cargo Norway domestic</t>
-  </si>
-  <si>
-    <t>Stykkgods til bedrift</t>
-  </si>
-  <si>
-    <t>5100</t>
-  </si>
-  <si>
-    <t>Pall til bedrift</t>
-  </si>
-  <si>
-    <t>5400</t>
   </si>
   <si>
     <t>Før 07:00 til bedrift</t>
@@ -1281,7 +1281,7 @@
         <v>23</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>23</v>
@@ -1316,13 +1316,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>39</v>
@@ -1369,16 +1369,16 @@
         <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>23</v>
@@ -1422,16 +1422,16 @@
         <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>23</v>
@@ -1469,19 +1469,19 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>21</v>
@@ -1508,16 +1508,16 @@
         <v>23</v>
       </c>
       <c r="N13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="P13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="Q13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14">
@@ -1528,13 +1528,13 @@
         <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>21</v>
@@ -1546,31 +1546,31 @@
         <v>23</v>
       </c>
       <c r="I14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="Q14" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="15">
@@ -1581,13 +1581,13 @@
         <v>25</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>21</v>
@@ -1599,31 +1599,31 @@
         <v>23</v>
       </c>
       <c r="I15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="P15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16">
@@ -1634,13 +1634,13 @@
         <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>34</v>
@@ -1667,16 +1667,16 @@
         <v>23</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="P16" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="Q16" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17">
@@ -1687,13 +1687,13 @@
         <v>25</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>34</v>
@@ -1705,31 +1705,31 @@
         <v>23</v>
       </c>
       <c r="I17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="P17" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="Q17" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18">
@@ -1740,13 +1740,13 @@
         <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>34</v>
@@ -1782,7 +1782,7 @@
         <v>22</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19">
@@ -1793,13 +1793,13 @@
         <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>34</v>
@@ -1811,28 +1811,28 @@
         <v>23</v>
       </c>
       <c r="I19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="P19" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>22</v>
@@ -1846,13 +1846,13 @@
         <v>25</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>34</v>
@@ -1882,13 +1882,13 @@
         <v>22</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21">
@@ -1899,13 +1899,13 @@
         <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>34</v>
@@ -1935,13 +1935,13 @@
         <v>22</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22">
@@ -1952,13 +1952,13 @@
         <v>25</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>34</v>
@@ -1988,13 +1988,13 @@
         <v>22</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23">
@@ -2005,13 +2005,13 @@
         <v>25</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>39</v>
@@ -2023,7 +2023,7 @@
         <v>23</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>23</v>
@@ -2041,13 +2041,13 @@
         <v>22</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24">
@@ -2058,13 +2058,13 @@
         <v>25</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>39</v>
@@ -2076,7 +2076,7 @@
         <v>23</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>23</v>
@@ -2094,13 +2094,13 @@
         <v>22</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25">
@@ -2111,16 +2111,16 @@
         <v>25</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="F25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>23</v>
@@ -2129,7 +2129,7 @@
         <v>23</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>23</v>
@@ -2147,13 +2147,13 @@
         <v>22</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26">
@@ -2164,16 +2164,16 @@
         <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="F26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>23</v>
@@ -2182,7 +2182,7 @@
         <v>23</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>23</v>
@@ -2200,30 +2200,30 @@
         <v>22</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="E27" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>34</v>
@@ -2270,13 +2270,13 @@
         <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="E28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>34</v>
@@ -2288,7 +2288,7 @@
         <v>23</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>23</v>
@@ -2438,7 +2438,7 @@
         <v>116</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>23</v>
@@ -2500,7 +2500,7 @@
         <v>22</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>23</v>
@@ -2518,13 +2518,13 @@
         <v>22</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33">
@@ -2553,7 +2553,7 @@
         <v>23</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>23</v>
@@ -2571,13 +2571,13 @@
         <v>22</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34">
@@ -2606,7 +2606,7 @@
         <v>23</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>23</v>
@@ -2624,13 +2624,13 @@
         <v>22</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35">
@@ -2659,7 +2659,7 @@
         <v>23</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>23</v>
@@ -2677,13 +2677,13 @@
         <v>22</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36">
@@ -2712,7 +2712,7 @@
         <v>23</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>23</v>
@@ -2730,13 +2730,13 @@
         <v>22</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37">
@@ -2765,7 +2765,7 @@
         <v>23</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>23</v>
@@ -2783,13 +2783,13 @@
         <v>22</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38">
@@ -2818,7 +2818,7 @@
         <v>23</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>23</v>
@@ -2836,13 +2836,13 @@
         <v>22</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39">
@@ -2871,7 +2871,7 @@
         <v>23</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>23</v>
@@ -2889,13 +2889,13 @@
         <v>22</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40">
@@ -2948,7 +2948,7 @@
         <v>22</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41">
@@ -3001,7 +3001,7 @@
         <v>22</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42">
@@ -3054,7 +3054,7 @@
         <v>22</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43">
@@ -3107,7 +3107,7 @@
         <v>22</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44">
@@ -3160,7 +3160,7 @@
         <v>22</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45">
@@ -3213,7 +3213,7 @@
         <v>22</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46">
@@ -3266,7 +3266,7 @@
         <v>22</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47">
@@ -3319,7 +3319,7 @@
         <v>22</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48">
@@ -3372,7 +3372,7 @@
         <v>22</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49">
@@ -3425,7 +3425,7 @@
         <v>22</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50">
@@ -3454,7 +3454,7 @@
         <v>23</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>23</v>
@@ -3478,7 +3478,7 @@
         <v>22</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51">
@@ -3525,13 +3525,13 @@
         <v>22</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52">
@@ -3578,10 +3578,10 @@
         <v>22</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q52" s="1" t="s">
         <v>22</v>
@@ -3631,10 +3631,10 @@
         <v>22</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q53" s="1" t="s">
         <v>22</v>
@@ -3684,10 +3684,10 @@
         <v>22</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q54" s="1" t="s">
         <v>22</v>
@@ -3737,10 +3737,10 @@
         <v>22</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q55" s="1" t="s">
         <v>22</v>
@@ -4037,7 +4037,7 @@
         <v>23</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>23</v>
@@ -4065,12 +4065,12 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="s">
+      <c r="A62" t="s" s="0">
         <v>211</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="s">
+      <c r="A63" t="s" s="0">
         <v>212</v>
       </c>
     </row>

</xml_diff>

<commit_message>
5200 in now supported in booking API
- also adding en translations
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="213">
   <si>
     <t>Service family</t>
   </si>
@@ -74,7 +74,7 @@
     <t>Main customer number</t>
   </si>
   <si>
-    <t>Pakke til hentested</t>
+    <t>Pickup parcel</t>
   </si>
   <si>
     <t>5800</t>
@@ -95,25 +95,25 @@
     <t/>
   </si>
   <si>
-    <t>Pakke levert hjem</t>
+    <t>Home delivery parcel</t>
   </si>
   <si>
     <t>5600</t>
   </si>
   <si>
-    <t>Pakke i postkassen</t>
+    <t>Mailbox parcel</t>
   </si>
   <si>
     <t>3584</t>
   </si>
   <si>
-    <t>Pakke i postkassen med RFID</t>
+    <t>Mailbox parcel with RFID</t>
   </si>
   <si>
     <t>3570</t>
   </si>
   <si>
-    <t>Pakke til bedrift</t>
+    <t>Business parcel</t>
   </si>
   <si>
     <t>5000</t>
@@ -122,13 +122,13 @@
     <t>B2B</t>
   </si>
   <si>
-    <t>Ekspress neste dag</t>
+    <t>Express next day</t>
   </si>
   <si>
     <t>4850</t>
   </si>
   <si>
-    <t>Retur fra hentested</t>
+    <t>Return from pick-up point</t>
   </si>
   <si>
     <t>9300</t>
@@ -137,22 +137,19 @@
     <t>B2C return</t>
   </si>
   <si>
-    <t>Retur til bedrift</t>
+    <t>Return parcel to business</t>
   </si>
   <si>
     <t>9350</t>
   </si>
   <si>
-    <t>C2B return</t>
-  </si>
-  <si>
-    <t>Retur pakke i postkassen</t>
+    <t>Return mailbox parcel</t>
   </si>
   <si>
     <t>9650</t>
   </si>
   <si>
-    <t>Retur pakke fra bedrift</t>
+    <t>Return business parcel</t>
   </si>
   <si>
     <t>9000</t>
@@ -161,7 +158,7 @@
     <t>B2B return</t>
   </si>
   <si>
-    <t>Returekspress</t>
+    <t>Return express</t>
   </si>
   <si>
     <t>9600</t>
@@ -332,13 +329,13 @@
     <t>Cargo Norway domestic</t>
   </si>
   <si>
-    <t>Stykkgods til bedrift</t>
+    <t>Business groupage</t>
   </si>
   <si>
     <t>5100</t>
   </si>
   <si>
-    <t>Pall til bedrift</t>
+    <t>Business pallet</t>
   </si>
   <si>
     <t>5400</t>
@@ -347,22 +344,19 @@
     <t>Customer setup</t>
   </si>
   <si>
-    <t>Før 07:00 til bedrift</t>
+    <t>Business before 07:00</t>
   </si>
   <si>
     <t>5200</t>
   </si>
   <si>
-    <t>5200*</t>
-  </si>
-  <si>
-    <t>Partigods til bedrift</t>
+    <t>Business partload</t>
   </si>
   <si>
     <t>5300</t>
   </si>
   <si>
-    <t>Retur stykkgods fra bedrift</t>
+    <t>Return business groupage</t>
   </si>
   <si>
     <t>9100</t>
@@ -608,7 +602,7 @@
     <t>Supply Base Logistics</t>
   </si>
   <si>
-    <t>Oljeekspressen</t>
+    <t>Oil Express</t>
   </si>
   <si>
     <t>OIL_EXPRESS</t>
@@ -641,7 +635,7 @@
     <t>3610*</t>
   </si>
   <si>
-    <t>Sporbar brevpakke bedrift</t>
+    <t>International Tracked Packet</t>
   </si>
   <si>
     <t>3630</t>
@@ -1272,7 +1266,7 @@
         <v>41</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>23</v>
@@ -1316,13 +1310,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>39</v>
@@ -1369,16 +1363,16 @@
         <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>23</v>
@@ -1422,16 +1416,16 @@
         <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>23</v>
@@ -1469,19 +1463,19 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>21</v>
@@ -1508,16 +1502,16 @@
         <v>23</v>
       </c>
       <c r="N13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="P13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="Q13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14">
@@ -1528,13 +1522,13 @@
         <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>21</v>
@@ -1546,31 +1540,31 @@
         <v>23</v>
       </c>
       <c r="I14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="Q14" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="15">
@@ -1581,13 +1575,13 @@
         <v>25</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>21</v>
@@ -1599,31 +1593,31 @@
         <v>23</v>
       </c>
       <c r="I15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="P15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16">
@@ -1634,13 +1628,13 @@
         <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>34</v>
@@ -1667,16 +1661,16 @@
         <v>23</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="P16" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="Q16" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17">
@@ -1687,13 +1681,13 @@
         <v>25</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>34</v>
@@ -1705,31 +1699,31 @@
         <v>23</v>
       </c>
       <c r="I17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="O17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="P17" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="Q17" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18">
@@ -1740,13 +1734,13 @@
         <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>34</v>
@@ -1782,7 +1776,7 @@
         <v>22</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19">
@@ -1793,13 +1787,13 @@
         <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>34</v>
@@ -1811,28 +1805,28 @@
         <v>23</v>
       </c>
       <c r="I19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="P19" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>22</v>
@@ -1846,13 +1840,13 @@
         <v>25</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>34</v>
@@ -1882,13 +1876,13 @@
         <v>22</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21">
@@ -1899,13 +1893,13 @@
         <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>34</v>
@@ -1935,13 +1929,13 @@
         <v>22</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22">
@@ -1952,13 +1946,13 @@
         <v>25</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>34</v>
@@ -1988,13 +1982,13 @@
         <v>22</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23">
@@ -2005,13 +1999,13 @@
         <v>25</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>39</v>
@@ -2023,7 +2017,7 @@
         <v>23</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>23</v>
@@ -2041,13 +2035,13 @@
         <v>22</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24">
@@ -2058,13 +2052,13 @@
         <v>25</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>39</v>
@@ -2076,7 +2070,7 @@
         <v>23</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>23</v>
@@ -2094,13 +2088,13 @@
         <v>22</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25">
@@ -2111,16 +2105,16 @@
         <v>25</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="F25" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>23</v>
@@ -2129,7 +2123,7 @@
         <v>23</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>23</v>
@@ -2147,13 +2141,13 @@
         <v>22</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26">
@@ -2164,16 +2158,16 @@
         <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="F26" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>23</v>
@@ -2182,7 +2176,7 @@
         <v>23</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>23</v>
@@ -2200,30 +2194,30 @@
         <v>22</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="E27" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>34</v>
@@ -2270,13 +2264,13 @@
         <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="E28" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>34</v>
@@ -2288,7 +2282,7 @@
         <v>23</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>23</v>
@@ -2323,13 +2317,13 @@
         <v>25</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="E29" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>34</v>
@@ -2338,7 +2332,7 @@
         <v>22</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>22</v>
@@ -2376,13 +2370,13 @@
         <v>25</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>34</v>
@@ -2429,16 +2423,16 @@
         <v>25</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>23</v>
@@ -2476,19 +2470,19 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>21</v>
@@ -2500,7 +2494,7 @@
         <v>22</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>23</v>
@@ -2518,13 +2512,13 @@
         <v>22</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33">
@@ -2535,13 +2529,13 @@
         <v>25</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>21</v>
@@ -2553,7 +2547,7 @@
         <v>23</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>23</v>
@@ -2571,13 +2565,13 @@
         <v>22</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34">
@@ -2588,13 +2582,13 @@
         <v>25</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>21</v>
@@ -2606,7 +2600,7 @@
         <v>23</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>23</v>
@@ -2624,13 +2618,13 @@
         <v>22</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35">
@@ -2641,13 +2635,13 @@
         <v>25</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>21</v>
@@ -2659,7 +2653,7 @@
         <v>23</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>23</v>
@@ -2677,13 +2671,13 @@
         <v>22</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36">
@@ -2694,13 +2688,13 @@
         <v>25</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>21</v>
@@ -2712,7 +2706,7 @@
         <v>23</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>23</v>
@@ -2730,13 +2724,13 @@
         <v>22</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37">
@@ -2747,13 +2741,13 @@
         <v>25</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>39</v>
@@ -2765,7 +2759,7 @@
         <v>23</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>23</v>
@@ -2783,13 +2777,13 @@
         <v>22</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38">
@@ -2800,13 +2794,13 @@
         <v>25</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>39</v>
@@ -2818,7 +2812,7 @@
         <v>23</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>23</v>
@@ -2836,13 +2830,13 @@
         <v>22</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39">
@@ -2853,13 +2847,13 @@
         <v>25</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>39</v>
@@ -2871,7 +2865,7 @@
         <v>23</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>23</v>
@@ -2889,34 +2883,34 @@
         <v>22</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="G40" s="1" t="s">
         <v>22</v>
       </c>
@@ -2948,7 +2942,7 @@
         <v>22</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41">
@@ -2959,16 +2953,16 @@
         <v>25</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="F41" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>22</v>
@@ -3001,7 +2995,7 @@
         <v>22</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42">
@@ -3012,16 +3006,16 @@
         <v>25</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="F42" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>22</v>
@@ -3054,7 +3048,7 @@
         <v>22</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43">
@@ -3065,16 +3059,16 @@
         <v>25</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="F43" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>22</v>
@@ -3107,7 +3101,7 @@
         <v>22</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44">
@@ -3118,16 +3112,16 @@
         <v>25</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="F44" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>22</v>
@@ -3160,7 +3154,7 @@
         <v>22</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45">
@@ -3171,16 +3165,16 @@
         <v>25</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="F45" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>22</v>
@@ -3213,7 +3207,7 @@
         <v>22</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46">
@@ -3224,16 +3218,16 @@
         <v>25</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="F46" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>22</v>
@@ -3266,7 +3260,7 @@
         <v>22</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47">
@@ -3277,16 +3271,16 @@
         <v>25</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="F47" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>22</v>
@@ -3319,7 +3313,7 @@
         <v>22</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48">
@@ -3330,16 +3324,16 @@
         <v>25</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="F48" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>22</v>
@@ -3372,7 +3366,7 @@
         <v>22</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49">
@@ -3383,16 +3377,16 @@
         <v>25</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="F49" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>22</v>
@@ -3425,7 +3419,7 @@
         <v>22</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50">
@@ -3436,16 +3430,16 @@
         <v>25</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>22</v>
@@ -3454,7 +3448,7 @@
         <v>23</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>23</v>
@@ -3478,7 +3472,7 @@
         <v>22</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51">
@@ -3489,16 +3483,16 @@
         <v>25</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F51" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>22</v>
@@ -3525,13 +3519,13 @@
         <v>22</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52">
@@ -3542,16 +3536,16 @@
         <v>25</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="F52" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>22</v>
@@ -3578,10 +3572,10 @@
         <v>22</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q52" s="1" t="s">
         <v>22</v>
@@ -3595,16 +3589,16 @@
         <v>25</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="F53" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>22</v>
@@ -3631,10 +3625,10 @@
         <v>22</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q53" s="1" t="s">
         <v>22</v>
@@ -3648,16 +3642,16 @@
         <v>25</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="F54" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>22</v>
@@ -3684,10 +3678,10 @@
         <v>22</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q54" s="1" t="s">
         <v>22</v>
@@ -3701,16 +3695,16 @@
         <v>25</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>189</v>
-      </c>
       <c r="F55" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>22</v>
@@ -3737,10 +3731,10 @@
         <v>22</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q55" s="1" t="s">
         <v>22</v>
@@ -3748,19 +3742,19 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C56" s="1" t="s">
+      <c r="E56" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>34</v>
@@ -3790,10 +3784,10 @@
         <v>22</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="Q56" s="1" t="s">
         <v>22</v>
@@ -3801,19 +3795,19 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="D57" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>34</v>
@@ -3854,22 +3848,22 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="F58" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>22</v>
@@ -3913,16 +3907,16 @@
         <v>25</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>204</v>
-      </c>
       <c r="F59" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>22</v>
@@ -3966,16 +3960,16 @@
         <v>25</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="F60" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>22</v>
@@ -4019,16 +4013,16 @@
         <v>25</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>22</v>
@@ -4037,7 +4031,7 @@
         <v>23</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>23</v>
@@ -4058,7 +4052,7 @@
         <v>24</v>
       </c>
       <c r="P61" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="Q61" s="1" t="s">
         <v>22</v>
@@ -4066,22 +4060,22 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="1">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="1">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove support for 0336 to Slovakia and the UK
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -272,7 +272,7 @@
     <t>BUSINESS_PALLET</t>
   </si>
   <si>
-    <t>NO, SE, DK, FI, AT, AX, BE, CH, CZ, DE, EE, ES, FO, FR, GB, GL, GR, HU, IE, IS, IT, LT, LU, LV, NL, PL, PT, SI, SK</t>
+    <t>NO, SE, DK, FI, AT, AX, BE, CH, CZ, DE, EE, ES, FO, FR, GL, GR, HU, IE, IS, IT, LT, LU, LV, NL, PL, PT, SI</t>
   </si>
   <si>
     <t>Business Pallet (1/2 pallet)</t>
@@ -822,7 +822,7 @@
     <col min="13" max="13" width="11.2890625" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="21.28125" customWidth="true" bestFit="true"/>
     <col min="15" max="15" width="18.5546875" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="107.359375" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="99.73828125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Remove 'customer setup' for 3630
- also adding some leftover unrelated changes (stemming from booking/checkout service-country-vas-common lib changes)
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -693,96 +693,96 @@
     </border>
     <border>
       <left>
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </left>
     </border>
     <border>
       <left>
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </left>
       <right>
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </right>
     </border>
     <border>
       <left>
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </left>
       <right>
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </right>
       <top>
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </top>
     </border>
     <border>
       <left>
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </left>
       <right>
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </right>
       <top>
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom>
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </left>
       <right>
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </right>
       <top>
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom>
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </left>
       <right>
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </right>
       <top>
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </right>
       <top>
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="000000"/>
+        <color rgb="FF000000"/>
       </bottom>
     </border>
   </borders>
@@ -807,22 +807,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="66.99609375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="29.66015625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="35.046875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="14.015625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="35.31640625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="12.3125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="9.11328125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="9.58203125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="17.609375" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="16.87109375" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="10.75390625" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="18.28125" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="11.2890625" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="21.28125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="18.5546875" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="99.73828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="57.42578125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="25.421875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="30.0390625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.01171875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="30.26953125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="10.55078125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="7.8125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="8.21484375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="15.09375" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="14.4609375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="9.21875" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="15.66796875" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="9.67578125" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="18.23828125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="15.90234375" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="85.4921875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4031,7 +4031,7 @@
         <v>23</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>108</v>
+        <v>22</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
hide bring pack on dev-site
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Booking &amp; SG API" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$64</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="207">
   <si>
     <t>Service family</t>
   </si>
@@ -615,24 +615,6 @@
   </si>
   <si>
     <t>MAIL*</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
-    <t>3609</t>
-  </si>
-  <si>
-    <t>3609*</t>
-  </si>
-  <si>
-    <t>Registered</t>
-  </si>
-  <si>
-    <t>3610</t>
-  </si>
-  <si>
-    <t>3610*</t>
   </si>
   <si>
     <t>International Tracked Packet</t>
@@ -798,7 +780,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Q65"/>
+  <dimension ref="A1:Q63"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -808,7 +790,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="57.42578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="25.421875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="22.19921875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="30.0390625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.01171875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="30.26953125" customWidth="true" bestFit="true"/>
@@ -3745,7 +3727,7 @@
         <v>188</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>188</v>
+        <v>18</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>189</v>
@@ -3913,7 +3895,7 @@
         <v>201</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>143</v>
@@ -3922,7 +3904,7 @@
         <v>22</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>22</v>
@@ -3943,143 +3925,37 @@
         <v>22</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>22</v>
+        <v>202</v>
       </c>
       <c r="Q59" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C60" s="1" t="s">
+      <c r="A60" t="s" s="0">
         <v>203</v>
       </c>
-      <c r="D60" s="1" t="s">
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="E60" s="1" t="s">
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="1">
         <v>205</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J60" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K60" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q60" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C61" s="1" t="s">
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="1">
         <v>206</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J61" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K61" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O61" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P61" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="Q61" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s" s="0">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s" s="0">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s" s="1">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s" s="1">
-        <v>212</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P66"/>
+  <autoFilter ref="A1:P64"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove most Express services from docs
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Booking &amp; SG API" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$60</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="195">
   <si>
     <t>Service family</t>
   </si>
@@ -545,42 +545,6 @@
     <t>EXPRESS_NORDIC_SAME_DAY</t>
   </si>
   <si>
-    <t>Express International 09:00</t>
-  </si>
-  <si>
-    <t>3337</t>
-  </si>
-  <si>
-    <t>EXPRESS_INTERNATIONAL_0900</t>
-  </si>
-  <si>
-    <t>Express International 12:00</t>
-  </si>
-  <si>
-    <t>3338</t>
-  </si>
-  <si>
-    <t>EXPRESS_INTERNATIONAL_1200</t>
-  </si>
-  <si>
-    <t>Express International</t>
-  </si>
-  <si>
-    <t>3339</t>
-  </si>
-  <si>
-    <t>EXPRESS_INTERNATIONAL</t>
-  </si>
-  <si>
-    <t>Express Economy</t>
-  </si>
-  <si>
-    <t>3340</t>
-  </si>
-  <si>
-    <t>EXPRESS_ECONOMY</t>
-  </si>
-  <si>
     <t>Cargo Norway international</t>
   </si>
   <si>
@@ -615,24 +579,6 @@
   </si>
   <si>
     <t>MAIL*</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
-    <t>3609</t>
-  </si>
-  <si>
-    <t>3609*</t>
-  </si>
-  <si>
-    <t>Registered</t>
-  </si>
-  <si>
-    <t>3610</t>
-  </si>
-  <si>
-    <t>3610*</t>
   </si>
   <si>
     <t>International Tracked Packet</t>
@@ -798,7 +744,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Q65"/>
+  <dimension ref="A1:Q59"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -807,22 +753,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="57.42578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="25.421875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="30.0390625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.01171875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="30.26953125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="10.55078125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="7.8125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="8.21484375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="15.09375" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="14.4609375" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="9.21875" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="15.66796875" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="9.67578125" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="18.23828125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="15.90234375" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="85.4921875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="57.79296875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="22.33984375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="30.23046875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.08984375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="30.46484375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="10.62109375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="7.859375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="8.265625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="15.1875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="14.5546875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="9.27734375" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="15.76953125" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="9.73828125" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="18.35546875" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="16.00390625" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="86.03515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3530,22 +3476,22 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>25</v>
+        <v>176</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>143</v>
+        <v>34</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>22</v>
@@ -3563,19 +3509,19 @@
         <v>23</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N52" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>66</v>
+        <v>180</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="Q52" s="1" t="s">
         <v>22</v>
@@ -3583,22 +3529,22 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>25</v>
+        <v>181</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>25</v>
+        <v>182</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>143</v>
+        <v>34</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>22</v>
@@ -3613,7 +3559,7 @@
         <v>23</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L53" s="1" t="s">
         <v>22</v>
@@ -3625,30 +3571,30 @@
         <v>22</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>143</v>
@@ -3657,7 +3603,7 @@
         <v>22</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>22</v>
@@ -3678,13 +3624,13 @@
         <v>22</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55">
@@ -3695,13 +3641,13 @@
         <v>25</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>143</v>
@@ -3725,361 +3671,43 @@
         <v>22</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N55" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>60</v>
+        <v>190</v>
       </c>
       <c r="Q55" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E56" s="1" t="s">
+      <c r="A56" t="s" s="0">
         <v>191</v>
       </c>
-      <c r="F56" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J56" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M56" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N56" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O56" s="1" t="s">
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
         <v>192</v>
       </c>
-      <c r="P56" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q56" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="s">
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="1">
         <v>193</v>
       </c>
-      <c r="B57" s="1" t="s">
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="1">
         <v>194</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J57" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M57" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q57" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J58" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K58" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M58" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q58" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J59" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K59" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q59" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J60" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K60" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q60" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J61" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K61" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O61" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P61" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="Q61" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s" s="0">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s" s="0">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s" s="1">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s" s="1">
-        <v>212</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P66"/>
+  <autoFilter ref="A1:P60"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update services json and xls with environmental data
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -1766,7 +1766,7 @@
         <v>23</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>60</v>
@@ -2190,7 +2190,7 @@
         <v>23</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>22</v>
@@ -2243,7 +2243,7 @@
         <v>23</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O28" s="1" t="s">
         <v>22</v>
@@ -2455,7 +2455,7 @@
         <v>23</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O32" s="1" t="s">
         <v>66</v>
@@ -2508,7 +2508,7 @@
         <v>23</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O33" s="1" t="s">
         <v>66</v>
@@ -2561,7 +2561,7 @@
         <v>23</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O34" s="1" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
Update 1288 VAS rules and new receiving country for 3630
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Karoline.Seljebotn@posten.no/projects/bring/developer-site/static/services/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4206A8AD-B762-064E-AEEC-EB498D5BF854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Booking &amp; SG API" r:id="rId3" sheetId="1"/>
+    <sheet name="Booking &amp; SG API" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Booking &amp; SG API'!$A$1:$P$60</definedName>
   </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -587,7 +595,7 @@
     <t>3630</t>
   </si>
   <si>
-    <t>SE, DK, FI, AT, BE, CH, CZ, DE, EE, FR, GB, HR, HU, IE, IS, LT, LU, LV, NL, PL, SI, SK</t>
+    <t>SE, DK, FI, AT, BE, CH, CZ, DE, EE, FR, GB, HR, HU, IE, IS, IT, LT, LU, LV, NL, PL, SI, SK</t>
   </si>
   <si>
     <t>* Only supported in Shipping Guide API</t>
@@ -605,20 +613,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
       <name val="Calibri"/>
-      <sz val="12.0"/>
-      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -626,96 +633,16 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
-    </border>
-    <border>
-      <left>
-        <color rgb="FF000000"/>
-      </left>
-    </border>
-    <border>
-      <left>
-        <color rgb="FF000000"/>
-      </left>
-      <right>
-        <color rgb="FF000000"/>
-      </right>
-    </border>
-    <border>
-      <left>
-        <color rgb="FF000000"/>
-      </left>
-      <right>
-        <color rgb="FF000000"/>
-      </right>
-      <top>
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left>
-        <color rgb="FF000000"/>
-      </left>
-      <right>
-        <color rgb="FF000000"/>
-      </right>
-      <top>
-        <color rgb="FF000000"/>
-      </top>
-      <bottom>
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right>
-        <color rgb="FF000000"/>
-      </right>
-      <top>
-        <color rgb="FF000000"/>
-      </top>
-      <bottom>
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right>
-        <color rgb="FF000000"/>
-      </right>
-      <top>
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top>
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -730,6 +657,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -737,41 +665,369 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="0E2841"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E8E8E8"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="156082"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="E97132"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="196B24"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="0F9ED5"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="A02B93"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="4EA72E"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="467886"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="96607D"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true">
-      <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54:XFD54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57.79296875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="22.33984375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="30.23046875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.08984375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="30.46484375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="10.62109375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="7.859375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="8.265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="15.1875" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="14.5546875" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="9.27734375" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="15.76953125" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="9.73828125" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="18.35546875" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="16.00390625" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="86.03515625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="57.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="86" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -824,7 +1080,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -877,7 +1133,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -930,7 +1186,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -983,7 +1239,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1036,7 +1292,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1089,7 +1345,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1142,7 +1398,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -1195,7 +1451,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -1248,7 +1504,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1301,7 +1557,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -1354,7 +1610,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -1407,7 +1663,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -1460,7 +1716,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1513,7 +1769,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -1566,7 +1822,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1619,7 +1875,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -1672,7 +1928,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
@@ -1725,7 +1981,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -1778,7 +2034,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -1831,7 +2087,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -1884,7 +2140,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1937,7 +2193,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1990,7 +2246,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -2043,7 +2299,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -2096,7 +2352,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -2149,7 +2405,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>103</v>
       </c>
@@ -2202,7 +2458,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -2255,7 +2511,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -2308,7 +2564,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -2361,7 +2617,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -2414,7 +2670,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>115</v>
       </c>
@@ -2467,7 +2723,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>25</v>
       </c>
@@ -2520,7 +2776,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
@@ -2573,7 +2829,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>25</v>
       </c>
@@ -2626,7 +2882,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>25</v>
       </c>
@@ -2679,7 +2935,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>25</v>
       </c>
@@ -2732,7 +2988,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>25</v>
       </c>
@@ -2785,7 +3041,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>25</v>
       </c>
@@ -2838,7 +3094,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>139</v>
       </c>
@@ -2891,7 +3147,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
@@ -2944,7 +3200,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>25</v>
       </c>
@@ -2997,7 +3253,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
@@ -3050,7 +3306,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>25</v>
       </c>
@@ -3103,7 +3359,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>25</v>
       </c>
@@ -3156,7 +3412,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>25</v>
       </c>
@@ -3209,7 +3465,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -3262,7 +3518,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>25</v>
       </c>
@@ -3315,7 +3571,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>25</v>
       </c>
@@ -3368,7 +3624,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>25</v>
       </c>
@@ -3421,7 +3677,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>25</v>
       </c>
@@ -3474,7 +3730,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>176</v>
       </c>
@@ -3527,7 +3783,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>181</v>
       </c>
@@ -3580,7 +3836,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>185</v>
       </c>
@@ -3633,7 +3889,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>25</v>
       </c>
@@ -3686,28 +3942,28 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="s" s="0">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="s" s="0">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" t="s" s="1">
+    <row r="58" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="s" s="1">
+    <row r="59" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>194</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P60"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <autoFilter ref="A1:P60" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update 1288 VAS rules and new receiving country for 3630 (#1718)
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Karoline.Seljebotn@posten.no/projects/bring/developer-site/static/services/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4206A8AD-B762-064E-AEEC-EB498D5BF854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Booking &amp; SG API" r:id="rId3" sheetId="1"/>
+    <sheet name="Booking &amp; SG API" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Booking &amp; SG API'!$A$1:$P$60</definedName>
   </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -587,7 +595,7 @@
     <t>3630</t>
   </si>
   <si>
-    <t>SE, DK, FI, AT, BE, CH, CZ, DE, EE, FR, GB, HR, HU, IE, IS, LT, LU, LV, NL, PL, SI, SK</t>
+    <t>SE, DK, FI, AT, BE, CH, CZ, DE, EE, FR, GB, HR, HU, IE, IS, IT, LT, LU, LV, NL, PL, SI, SK</t>
   </si>
   <si>
     <t>* Only supported in Shipping Guide API</t>
@@ -605,20 +613,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
       <name val="Calibri"/>
-      <sz val="12.0"/>
-      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -626,96 +633,16 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
-    </border>
-    <border>
-      <left>
-        <color rgb="FF000000"/>
-      </left>
-    </border>
-    <border>
-      <left>
-        <color rgb="FF000000"/>
-      </left>
-      <right>
-        <color rgb="FF000000"/>
-      </right>
-    </border>
-    <border>
-      <left>
-        <color rgb="FF000000"/>
-      </left>
-      <right>
-        <color rgb="FF000000"/>
-      </right>
-      <top>
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left>
-        <color rgb="FF000000"/>
-      </left>
-      <right>
-        <color rgb="FF000000"/>
-      </right>
-      <top>
-        <color rgb="FF000000"/>
-      </top>
-      <bottom>
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right>
-        <color rgb="FF000000"/>
-      </right>
-      <top>
-        <color rgb="FF000000"/>
-      </top>
-      <bottom>
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right>
-        <color rgb="FF000000"/>
-      </right>
-      <top>
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top>
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -730,6 +657,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -737,41 +665,369 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="0E2841"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E8E8E8"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="156082"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="E97132"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="196B24"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="0F9ED5"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="A02B93"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="4EA72E"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="467886"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="96607D"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true">
-      <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54:XFD54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57.79296875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="22.33984375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="30.23046875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.08984375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="30.46484375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="10.62109375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="7.859375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="8.265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="15.1875" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="14.5546875" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="9.27734375" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="15.76953125" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="9.73828125" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="18.35546875" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="16.00390625" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="86.03515625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="57.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="86" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -824,7 +1080,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -877,7 +1133,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -930,7 +1186,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -983,7 +1239,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1036,7 +1292,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1089,7 +1345,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1142,7 +1398,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -1195,7 +1451,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -1248,7 +1504,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1301,7 +1557,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -1354,7 +1610,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -1407,7 +1663,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -1460,7 +1716,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1513,7 +1769,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -1566,7 +1822,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1619,7 +1875,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -1672,7 +1928,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
@@ -1725,7 +1981,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -1778,7 +2034,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -1831,7 +2087,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -1884,7 +2140,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1937,7 +2193,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1990,7 +2246,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -2043,7 +2299,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -2096,7 +2352,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -2149,7 +2405,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>103</v>
       </c>
@@ -2202,7 +2458,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -2255,7 +2511,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -2308,7 +2564,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -2361,7 +2617,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -2414,7 +2670,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>115</v>
       </c>
@@ -2467,7 +2723,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>25</v>
       </c>
@@ -2520,7 +2776,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
@@ -2573,7 +2829,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>25</v>
       </c>
@@ -2626,7 +2882,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>25</v>
       </c>
@@ -2679,7 +2935,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>25</v>
       </c>
@@ -2732,7 +2988,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>25</v>
       </c>
@@ -2785,7 +3041,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>25</v>
       </c>
@@ -2838,7 +3094,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>139</v>
       </c>
@@ -2891,7 +3147,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
@@ -2944,7 +3200,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>25</v>
       </c>
@@ -2997,7 +3253,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
@@ -3050,7 +3306,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>25</v>
       </c>
@@ -3103,7 +3359,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>25</v>
       </c>
@@ -3156,7 +3412,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>25</v>
       </c>
@@ -3209,7 +3465,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -3262,7 +3518,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>25</v>
       </c>
@@ -3315,7 +3571,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>25</v>
       </c>
@@ -3368,7 +3624,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>25</v>
       </c>
@@ -3421,7 +3677,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>25</v>
       </c>
@@ -3474,7 +3730,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>176</v>
       </c>
@@ -3527,7 +3783,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>181</v>
       </c>
@@ -3580,7 +3836,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>185</v>
       </c>
@@ -3633,7 +3889,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>25</v>
       </c>
@@ -3686,28 +3942,28 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="s" s="0">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="s" s="0">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" t="s" s="1">
+    <row r="58" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="s" s="1">
+    <row r="59" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>194</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P60"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <autoFilter ref="A1:P60" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Update 1288 VAS rules and new receiving country for 3630 (#1718)"
This reverts commit fe6ec0d5bfd26801ecc36fd501f3c665e6ffb25a.
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -1,24 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Karoline.Seljebotn@posten.no/projects/bring/developer-site/static/services/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4206A8AD-B762-064E-AEEC-EB498D5BF854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Booking &amp; SG API" sheetId="1" r:id="rId1"/>
+    <sheet name="Booking &amp; SG API" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Booking &amp; SG API'!$A$1:$P$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$60</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -595,7 +587,7 @@
     <t>3630</t>
   </si>
   <si>
-    <t>SE, DK, FI, AT, BE, CH, CZ, DE, EE, FR, GB, HR, HU, IE, IS, IT, LT, LU, LV, NL, PL, SI, SK</t>
+    <t>SE, DK, FI, AT, BE, CH, CZ, DE, EE, FR, GB, HR, HU, IE, IS, LT, LU, LV, NL, PL, SI, SK</t>
   </si>
   <si>
     <t>* Only supported in Shipping Guide API</t>
@@ -613,19 +605,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color indexed="8"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
       <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -633,16 +626,96 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="darkGray"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
+      <left>
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left>
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left>
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom>
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom>
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -657,7 +730,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -665,369 +737,41 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="0E2841"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="156082"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="E97132"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="196B24"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="A02B93"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="4EA72E"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="467886"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="96607D"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A54:XFD54"/>
+    <sheetView workbookViewId="0" tabSelected="true">
+      <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="57.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="86" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.79296875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="22.33984375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="30.23046875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.08984375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="30.46484375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="10.62109375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="7.859375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="8.265625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="15.1875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="14.5546875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="9.27734375" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="15.76953125" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="9.73828125" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="18.35546875" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="16.00390625" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="86.03515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1080,7 +824,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1133,7 +877,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -1186,7 +930,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -1239,7 +983,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1292,7 +1036,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1345,7 +1089,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1398,7 +1142,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -1451,7 +1195,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -1504,7 +1248,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1557,7 +1301,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -1610,7 +1354,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -1663,7 +1407,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -1716,7 +1460,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1769,7 +1513,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -1822,7 +1566,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1875,7 +1619,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -1928,7 +1672,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
@@ -1981,7 +1725,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -2034,7 +1778,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -2087,7 +1831,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -2140,7 +1884,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -2193,7 +1937,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -2246,7 +1990,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -2299,7 +2043,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -2352,7 +2096,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -2405,7 +2149,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="A27" s="1" t="s">
         <v>103</v>
       </c>
@@ -2458,7 +2202,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -2511,7 +2255,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -2564,7 +2308,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -2617,7 +2361,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -2670,7 +2414,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="A32" s="1" t="s">
         <v>115</v>
       </c>
@@ -2723,7 +2467,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="33">
       <c r="A33" s="1" t="s">
         <v>25</v>
       </c>
@@ -2776,7 +2520,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="34">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
@@ -2829,7 +2573,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="35">
       <c r="A35" s="1" t="s">
         <v>25</v>
       </c>
@@ -2882,7 +2626,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="36">
       <c r="A36" s="1" t="s">
         <v>25</v>
       </c>
@@ -2935,7 +2679,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="37">
       <c r="A37" s="1" t="s">
         <v>25</v>
       </c>
@@ -2988,7 +2732,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="38">
       <c r="A38" s="1" t="s">
         <v>25</v>
       </c>
@@ -3041,7 +2785,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="39">
       <c r="A39" s="1" t="s">
         <v>25</v>
       </c>
@@ -3094,7 +2838,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="40">
       <c r="A40" s="1" t="s">
         <v>139</v>
       </c>
@@ -3147,7 +2891,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="41">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
@@ -3200,7 +2944,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="42">
       <c r="A42" s="1" t="s">
         <v>25</v>
       </c>
@@ -3253,7 +2997,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="43">
       <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
@@ -3306,7 +3050,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="44">
       <c r="A44" s="1" t="s">
         <v>25</v>
       </c>
@@ -3359,7 +3103,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="45">
       <c r="A45" s="1" t="s">
         <v>25</v>
       </c>
@@ -3412,7 +3156,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="46">
       <c r="A46" s="1" t="s">
         <v>25</v>
       </c>
@@ -3465,7 +3209,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="47">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -3518,7 +3262,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="48">
       <c r="A48" s="1" t="s">
         <v>25</v>
       </c>
@@ -3571,7 +3315,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="49">
       <c r="A49" s="1" t="s">
         <v>25</v>
       </c>
@@ -3624,7 +3368,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="50">
       <c r="A50" s="1" t="s">
         <v>25</v>
       </c>
@@ -3677,7 +3421,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="51">
       <c r="A51" s="1" t="s">
         <v>25</v>
       </c>
@@ -3730,7 +3474,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="52">
       <c r="A52" s="1" t="s">
         <v>176</v>
       </c>
@@ -3783,7 +3527,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="53">
       <c r="A53" s="1" t="s">
         <v>181</v>
       </c>
@@ -3836,7 +3580,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="54">
       <c r="A54" s="1" t="s">
         <v>185</v>
       </c>
@@ -3889,7 +3633,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="55">
       <c r="A55" s="1" t="s">
         <v>25</v>
       </c>
@@ -3942,28 +3686,28 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="56">
+      <c r="A56" t="s" s="0">
         <v>191</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="57">
+      <c r="A57" t="s" s="0">
         <v>192</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+    <row r="58">
+      <c r="A58" t="s" s="1">
         <v>193</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+    <row r="59">
+      <c r="A59" t="s" s="1">
         <v>194</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P60" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <autoFilter ref="A1:P60"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Update 1288 VAS rules and new receiving country for 3630 (#1718)" (#1720)
This reverts commit fe6ec0d5bfd26801ecc36fd501f3c665e6ffb25a.
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -1,24 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Karoline.Seljebotn@posten.no/projects/bring/developer-site/static/services/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4206A8AD-B762-064E-AEEC-EB498D5BF854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Booking &amp; SG API" sheetId="1" r:id="rId1"/>
+    <sheet name="Booking &amp; SG API" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Booking &amp; SG API'!$A$1:$P$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$60</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -595,7 +587,7 @@
     <t>3630</t>
   </si>
   <si>
-    <t>SE, DK, FI, AT, BE, CH, CZ, DE, EE, FR, GB, HR, HU, IE, IS, IT, LT, LU, LV, NL, PL, SI, SK</t>
+    <t>SE, DK, FI, AT, BE, CH, CZ, DE, EE, FR, GB, HR, HU, IE, IS, LT, LU, LV, NL, PL, SI, SK</t>
   </si>
   <si>
     <t>* Only supported in Shipping Guide API</t>
@@ -613,19 +605,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color indexed="8"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
       <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -633,16 +626,96 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="darkGray"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
+      <left>
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left>
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left>
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom>
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom>
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -657,7 +730,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -665,369 +737,41 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="0E2841"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="156082"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="E97132"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="196B24"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="A02B93"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="4EA72E"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="467886"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="96607D"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A54:XFD54"/>
+    <sheetView workbookViewId="0" tabSelected="true">
+      <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="57.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="86" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.79296875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="22.33984375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="30.23046875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.08984375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="30.46484375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="10.62109375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="7.859375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="8.265625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="15.1875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="14.5546875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="9.27734375" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="15.76953125" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="9.73828125" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="18.35546875" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="16.00390625" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="86.03515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1080,7 +824,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1133,7 +877,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -1186,7 +930,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -1239,7 +983,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1292,7 +1036,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1345,7 +1089,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1398,7 +1142,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -1451,7 +1195,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -1504,7 +1248,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1557,7 +1301,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -1610,7 +1354,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -1663,7 +1407,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -1716,7 +1460,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1769,7 +1513,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -1822,7 +1566,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1875,7 +1619,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -1928,7 +1672,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
@@ -1981,7 +1725,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -2034,7 +1778,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -2087,7 +1831,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -2140,7 +1884,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -2193,7 +1937,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -2246,7 +1990,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -2299,7 +2043,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -2352,7 +2096,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -2405,7 +2149,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="A27" s="1" t="s">
         <v>103</v>
       </c>
@@ -2458,7 +2202,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -2511,7 +2255,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -2564,7 +2308,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -2617,7 +2361,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -2670,7 +2414,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="A32" s="1" t="s">
         <v>115</v>
       </c>
@@ -2723,7 +2467,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="33">
       <c r="A33" s="1" t="s">
         <v>25</v>
       </c>
@@ -2776,7 +2520,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="34">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
@@ -2829,7 +2573,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="35">
       <c r="A35" s="1" t="s">
         <v>25</v>
       </c>
@@ -2882,7 +2626,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="36">
       <c r="A36" s="1" t="s">
         <v>25</v>
       </c>
@@ -2935,7 +2679,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="37">
       <c r="A37" s="1" t="s">
         <v>25</v>
       </c>
@@ -2988,7 +2732,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="38">
       <c r="A38" s="1" t="s">
         <v>25</v>
       </c>
@@ -3041,7 +2785,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="39">
       <c r="A39" s="1" t="s">
         <v>25</v>
       </c>
@@ -3094,7 +2838,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="40">
       <c r="A40" s="1" t="s">
         <v>139</v>
       </c>
@@ -3147,7 +2891,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="41">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
@@ -3200,7 +2944,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="42">
       <c r="A42" s="1" t="s">
         <v>25</v>
       </c>
@@ -3253,7 +2997,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="43">
       <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
@@ -3306,7 +3050,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="44">
       <c r="A44" s="1" t="s">
         <v>25</v>
       </c>
@@ -3359,7 +3103,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="45">
       <c r="A45" s="1" t="s">
         <v>25</v>
       </c>
@@ -3412,7 +3156,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="46">
       <c r="A46" s="1" t="s">
         <v>25</v>
       </c>
@@ -3465,7 +3209,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="47">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -3518,7 +3262,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="48">
       <c r="A48" s="1" t="s">
         <v>25</v>
       </c>
@@ -3571,7 +3315,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="49">
       <c r="A49" s="1" t="s">
         <v>25</v>
       </c>
@@ -3624,7 +3368,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="50">
       <c r="A50" s="1" t="s">
         <v>25</v>
       </c>
@@ -3677,7 +3421,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="51">
       <c r="A51" s="1" t="s">
         <v>25</v>
       </c>
@@ -3730,7 +3474,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="52">
       <c r="A52" s="1" t="s">
         <v>176</v>
       </c>
@@ -3783,7 +3527,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="53">
       <c r="A53" s="1" t="s">
         <v>181</v>
       </c>
@@ -3836,7 +3580,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="54">
       <c r="A54" s="1" t="s">
         <v>185</v>
       </c>
@@ -3889,7 +3633,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="55">
       <c r="A55" s="1" t="s">
         <v>25</v>
       </c>
@@ -3942,28 +3686,28 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="56">
+      <c r="A56" t="s" s="0">
         <v>191</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="57">
+      <c r="A57" t="s" s="0">
         <v>192</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+    <row r="58">
+      <c r="A58" t="s" s="1">
         <v>193</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+    <row r="59">
+      <c r="A59" t="s" s="1">
         <v>194</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P60" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <autoFilter ref="A1:P60"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Streamlining 1142 vs 1149: Updated Vas table
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Booking &amp; SG API" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$62</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="199">
   <si>
     <t>Service family</t>
   </si>
@@ -203,54 +203,54 @@
     <t>NO, SE, DK, FI, DE, EE, FO, GB, IS, NL</t>
   </si>
   <si>
+    <t>Home Delivery Parcel</t>
+  </si>
+  <si>
+    <t>0349</t>
+  </si>
+  <si>
+    <t>HOME_DELIVERY_PARCEL</t>
+  </si>
+  <si>
+    <t>NO, SE, DK</t>
+  </si>
+  <si>
+    <t>Business Parcel</t>
+  </si>
+  <si>
+    <t>0330</t>
+  </si>
+  <si>
+    <t>BUSINESS_PARCEL</t>
+  </si>
+  <si>
+    <t>SE, DK, FI</t>
+  </si>
+  <si>
+    <t>Business Parcel Bulk</t>
+  </si>
+  <si>
+    <t>0332</t>
+  </si>
+  <si>
+    <t>BUSINESS_PARCEL_BULK</t>
+  </si>
+  <si>
+    <t>SE, FI</t>
+  </si>
+  <si>
+    <t>Express Nordic 09:00</t>
+  </si>
+  <si>
+    <t>0335</t>
+  </si>
+  <si>
+    <t>EXPRESS_NORDIC_0900</t>
+  </si>
+  <si>
     <t>SE</t>
   </si>
   <si>
-    <t>Home Delivery Parcel</t>
-  </si>
-  <si>
-    <t>0349</t>
-  </si>
-  <si>
-    <t>HOME_DELIVERY_PARCEL</t>
-  </si>
-  <si>
-    <t>NO, SE, DK</t>
-  </si>
-  <si>
-    <t>Business Parcel</t>
-  </si>
-  <si>
-    <t>0330</t>
-  </si>
-  <si>
-    <t>BUSINESS_PARCEL</t>
-  </si>
-  <si>
-    <t>SE, DK, FI</t>
-  </si>
-  <si>
-    <t>Business Parcel Bulk</t>
-  </si>
-  <si>
-    <t>0332</t>
-  </si>
-  <si>
-    <t>BUSINESS_PARCEL_BULK</t>
-  </si>
-  <si>
-    <t>SE, FI</t>
-  </si>
-  <si>
-    <t>Express Nordic 09:00</t>
-  </si>
-  <si>
-    <t>0335</t>
-  </si>
-  <si>
-    <t>EXPRESS_NORDIC_0900</t>
-  </si>
-  <si>
     <t>Express Nordic 09:00 Bulk</t>
   </si>
   <si>
@@ -566,12 +566,15 @@
     <t>Supply Base Logistics</t>
   </si>
   <si>
-    <t>Oil Express</t>
-  </si>
-  <si>
     <t>OIL_EXPRESS</t>
   </si>
   <si>
+    <t>Project Logistics</t>
+  </si>
+  <si>
+    <t>PROJECT_LOGISTICS</t>
+  </si>
+  <si>
     <t>Mail</t>
   </si>
   <si>
@@ -587,7 +590,16 @@
     <t>3630</t>
   </si>
   <si>
-    <t>SE, DK, FI, AT, BE, CH, CZ, DE, EE, FR, GB, HR, HU, IE, IS, LT, LU, LV, NL, PL, SI, SK</t>
+    <t>SE, DK, FI, AT, BE, CH, CZ, DE, EE, FR, GB, HR, HU, IE, IS, IT, LT, LU, LV, NL, PL, SI, SK</t>
+  </si>
+  <si>
+    <t>Letter Packet</t>
+  </si>
+  <si>
+    <t>3639</t>
+  </si>
+  <si>
+    <t>NO, SE, DK, FI, AD, AE, AG, AI, AL, AM, AN, AO, AQ, AR, AS, AT, AU, AW, AX, AZ, BA, BB, BD, BE, BF, BG, BH, BI, BJ, BL, BM, BN, BO, BQ, BR, BS, BV, BW, BY, BZ, CA, CC, CD, CF, CG, CH, CI, CK, CL, CM, CN, CO, CR, CU, CV, CW, CX, CY, CZ, DE, DJ, DM, DO, DZ, EC, EE, EG, EH, ER, ES, ET, FJ, FK, FM, FO, FR, GA, GB, GD, GE, GF, GG, GH, GI, GL, GM, GN, GP, GQ, GR, GS, GT, GU, GW, GY, HK, HM, HN, HR, HT, HU, ID, IE, IM, IN, IO, IQ, IR, IS, IT, JE, JM, JO, JP, KE, KG, KH, KI, KM, KN, KP, KR, KW, KY, KZ, LA, LB, LC, LI, LK, LR, LS, LT, LU, LV, MA, MC, MD, ME, MF, MG, MH, MK, ML, MM, MN, MO, MP, MQ, MR, MS, MT, MU, MV, MW, MX, MY, MZ, NA, NC, NE, NF, NG, NI, NL, NP, NR, NU, NZ, OM, PA, PE, PF, PG, PH, PK, PL, PM, PN, PR, PS, PT, PW, PY, QA, RE, RO, RS, RU, RW, SA, SB, SC, SG, SH, SI, SJ, SK, SL, SM, SN, SO, SR, ST, SV, SX, SZ, TC, TD, TF, TG, TH, TJ, TK, TL, TM, TN, TO, TR, TT, TV, TW, TZ, UA, UG, UM, US, UY, UZ, VA, VC, VE, VG, VI, VN, VU, WF, WS, XK, YT, ZA, ZM, ZW</t>
   </si>
   <si>
     <t>* Only supported in Shipping Guide API</t>
@@ -744,7 +756,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Q59"/>
+  <dimension ref="A1:Q61"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -768,7 +780,7 @@
     <col min="13" max="13" width="9.73828125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="18.35546875" customWidth="true" bestFit="true"/>
     <col min="15" max="15" width="16.00390625" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="86.03515625" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="255.0" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1510,7 +1522,7 @@
         <v>61</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15">
@@ -1521,13 +1533,13 @@
         <v>25</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>21</v>
@@ -1554,7 +1566,7 @@
         <v>23</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>60</v>
@@ -1574,13 +1586,13 @@
         <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>34</v>
@@ -1607,7 +1619,7 @@
         <v>23</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>54</v>
@@ -1616,7 +1628,7 @@
         <v>55</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17">
@@ -1627,13 +1639,13 @@
         <v>25</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>34</v>
@@ -1669,7 +1681,7 @@
         <v>61</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18">
@@ -1680,13 +1692,13 @@
         <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>34</v>
@@ -1722,7 +1734,7 @@
         <v>22</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19">
@@ -1828,7 +1840,7 @@
         <v>85</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21">
@@ -1881,7 +1893,7 @@
         <v>54</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22">
@@ -1931,10 +1943,10 @@
         <v>60</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23">
@@ -2458,13 +2470,13 @@
         <v>24</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33">
@@ -2511,13 +2523,13 @@
         <v>24</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34">
@@ -2564,13 +2576,13 @@
         <v>24</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35">
@@ -2617,13 +2629,13 @@
         <v>22</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36">
@@ -2723,13 +2735,13 @@
         <v>22</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38">
@@ -2776,13 +2788,13 @@
         <v>22</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39">
@@ -2829,13 +2841,13 @@
         <v>22</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40">
@@ -3153,7 +3165,7 @@
         <v>22</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46">
@@ -3206,7 +3218,7 @@
         <v>22</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47">
@@ -3259,7 +3271,7 @@
         <v>22</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48">
@@ -3312,7 +3324,7 @@
         <v>22</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49">
@@ -3365,7 +3377,7 @@
         <v>22</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50">
@@ -3465,13 +3477,13 @@
         <v>22</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P51" s="1" t="s">
         <v>54</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52">
@@ -3535,13 +3547,13 @@
         <v>182</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>178</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>34</v>
@@ -3582,28 +3594,28 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>187</v>
-      </c>
       <c r="F54" s="1" t="s">
-        <v>143</v>
+        <v>34</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>22</v>
@@ -3612,7 +3624,7 @@
         <v>23</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L54" s="1" t="s">
         <v>22</v>
@@ -3624,30 +3636,30 @@
         <v>22</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>25</v>
+        <v>186</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>143</v>
@@ -3656,7 +3668,7 @@
         <v>22</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>22</v>
@@ -3671,43 +3683,149 @@
         <v>22</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N55" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q55" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P55" s="1" t="s">
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="Q55" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s" s="0">
+      <c r="E56" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P56" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="Q56" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="57">
-      <c r="A57" t="s" s="0">
+      <c r="A57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>192</v>
       </c>
+      <c r="D57" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O57" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q57" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="58">
-      <c r="A58" t="s" s="1">
-        <v>193</v>
+      <c r="A58" t="s" s="0">
+        <v>195</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="s" s="1">
-        <v>194</v>
+      <c r="A59" t="s" s="0">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="1">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="1">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P60"/>
+  <autoFilter ref="A1:P62"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add 3639 to service portfolio
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -1,21 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a2344567/projects/bring/developer-site/static/services/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2591A094-3BEE-F74D-B16F-8AD2591778AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Booking &amp; SG API" r:id="rId3" sheetId="1"/>
+    <sheet name="Booking &amp; SG API" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Booking &amp; SG API'!$A$1:$P$61</definedName>
   </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="198">
   <si>
     <t>Service family</t>
   </si>
@@ -600,25 +608,34 @@
   </si>
   <si>
     <t xml:space="preserve">Information applies to revised services only. </t>
+  </si>
+  <si>
+    <t>Letter Packet</t>
+  </si>
+  <si>
+    <t>3639</t>
+  </si>
+  <si>
+    <t>SE, DK, FI, AD, AE, AG, AI, AL, AM, AN, AO, AQ, AR, AS, AT, AU, AW, AX, AZ, BA, BB, BD, BE, BF, BG, BH, BI, BJ, BL, BM, BN, BO, BQ, BR, BS, BV, BW, BY, BZ, CA, CC, CD, CF, CG, CH, CI, CK, CL, CM, CN, CO, CR, CU, CV, CW, CX, CY, CZ, DE, DJ, DM, DO, DZ, EC, EE, EG, EH, ER, ES, ET, FJ, FK, FM, FO, FR, GA, GB, GD, GE, GF, GG, GH, GI, GL, GM, GN, GP, GQ, GR, GS, GT, GU, GW, GY, HK, HM, HN, HR, HT, HU, ID, IE, IM, IN, IO, IQ, IR, IS, IT, JE, JM, JO, JP, KE, KG, KH, KI, KM, KN, KP, KR, KW, KY, KZ, LA, LB, LC, LI, LK, LR, LS, LT, LU, LV, MA, MC, MD, ME, MF, MG, MH, MK, ML, MM, MN, MO, MP, MQ, MR, MS, MT, MU, MV, MW, MX, MY, MZ, NA, NC, NE, NF, NG, NI, NL, NP, NR, NU, NZ, OM, PA, PE, PF, PG, PH, PK, PL, PM, PN, PR, PS, PT, PW, PY, QA, RE, RO, RS, RU, RW, SA, SB, SC, SG, SH, SI, SJ, SK, SL, SM, SN, SO, SR, ST, SV, SX, SZ, TC, TD, TF, TG, TH, TJ, TK, TL, TM, TN, TO, TR, TT, TV, TW, TZ, UA, UG, UM, US, UY, UZ, VA, VC, VE, VG, VI, VN, VU, WF, WS, XK, YT, ZA, ZM, ZW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
       <name val="Calibri"/>
-      <sz val="12.0"/>
-      <b val="true"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -626,96 +643,16 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
-    </border>
-    <border>
-      <left>
-        <color rgb="FF000000"/>
-      </left>
-    </border>
-    <border>
-      <left>
-        <color rgb="FF000000"/>
-      </left>
-      <right>
-        <color rgb="FF000000"/>
-      </right>
-    </border>
-    <border>
-      <left>
-        <color rgb="FF000000"/>
-      </left>
-      <right>
-        <color rgb="FF000000"/>
-      </right>
-      <top>
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left>
-        <color rgb="FF000000"/>
-      </left>
-      <right>
-        <color rgb="FF000000"/>
-      </right>
-      <top>
-        <color rgb="FF000000"/>
-      </top>
-      <bottom>
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right>
-        <color rgb="FF000000"/>
-      </right>
-      <top>
-        <color rgb="FF000000"/>
-      </top>
-      <bottom>
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right>
-        <color rgb="FF000000"/>
-      </right>
-      <top>
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top>
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -730,6 +667,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -737,41 +675,349 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Q59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true">
-      <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P56" sqref="P56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57.79296875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="22.33984375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="30.23046875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.08984375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="30.46484375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="10.62109375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="7.859375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="8.265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="15.1875" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="14.5546875" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="9.27734375" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="15.76953125" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="9.73828125" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="18.35546875" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="16.00390625" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="86.03515625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="57.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="86" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -824,7 +1070,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -877,7 +1123,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -930,7 +1176,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -983,7 +1229,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1036,7 +1282,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1089,7 +1335,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1142,7 +1388,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -1195,7 +1441,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -1248,7 +1494,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1301,7 +1547,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -1354,7 +1600,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -1407,7 +1653,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -1460,7 +1706,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1513,7 +1759,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -1566,7 +1812,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1619,7 +1865,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -1672,7 +1918,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
@@ -1725,7 +1971,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -1778,7 +2024,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -1831,7 +2077,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -1884,7 +2130,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1937,7 +2183,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1990,7 +2236,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -2043,7 +2289,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -2096,7 +2342,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -2149,7 +2395,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>103</v>
       </c>
@@ -2202,7 +2448,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -2255,7 +2501,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -2308,7 +2554,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -2361,7 +2607,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -2414,7 +2660,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>115</v>
       </c>
@@ -2467,7 +2713,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>25</v>
       </c>
@@ -2520,7 +2766,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
@@ -2573,7 +2819,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>25</v>
       </c>
@@ -2626,7 +2872,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>25</v>
       </c>
@@ -2679,7 +2925,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>25</v>
       </c>
@@ -2732,7 +2978,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>25</v>
       </c>
@@ -2785,7 +3031,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>25</v>
       </c>
@@ -2838,7 +3084,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>139</v>
       </c>
@@ -2891,7 +3137,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
@@ -2944,7 +3190,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>25</v>
       </c>
@@ -2997,7 +3243,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
@@ -3050,7 +3296,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>25</v>
       </c>
@@ -3103,7 +3349,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>25</v>
       </c>
@@ -3156,7 +3402,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>25</v>
       </c>
@@ -3209,7 +3455,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -3262,7 +3508,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>25</v>
       </c>
@@ -3315,7 +3561,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>25</v>
       </c>
@@ -3368,7 +3614,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>25</v>
       </c>
@@ -3421,7 +3667,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>25</v>
       </c>
@@ -3474,7 +3720,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>176</v>
       </c>
@@ -3527,7 +3773,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>181</v>
       </c>
@@ -3580,7 +3826,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>185</v>
       </c>
@@ -3633,7 +3879,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>25</v>
       </c>
@@ -3686,28 +3932,81 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="s" s="0">
+    <row r="56" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P56" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q56" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="s" s="0">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" t="s" s="1">
+    <row r="59" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="s" s="1">
+    <row r="60" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>194</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P60"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <autoFilter ref="A1:P61" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Generated from latest Common-vas
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -1,29 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a2344567/projects/bring/developer-site/static/services/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2591A094-3BEE-F74D-B16F-8AD2591778AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Booking &amp; SG API" sheetId="1" r:id="rId1"/>
+    <sheet name="Booking &amp; SG API" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Booking &amp; SG API'!$A$1:$P$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$62</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="199">
   <si>
     <t>Service family</t>
   </si>
@@ -211,54 +203,54 @@
     <t>NO, SE, DK, FI, DE, EE, FO, GB, IS, NL</t>
   </si>
   <si>
+    <t>Home Delivery Parcel</t>
+  </si>
+  <si>
+    <t>0349</t>
+  </si>
+  <si>
+    <t>HOME_DELIVERY_PARCEL</t>
+  </si>
+  <si>
+    <t>NO, SE, DK</t>
+  </si>
+  <si>
+    <t>Business Parcel</t>
+  </si>
+  <si>
+    <t>0330</t>
+  </si>
+  <si>
+    <t>BUSINESS_PARCEL</t>
+  </si>
+  <si>
+    <t>SE, DK, FI</t>
+  </si>
+  <si>
+    <t>Business Parcel Bulk</t>
+  </si>
+  <si>
+    <t>0332</t>
+  </si>
+  <si>
+    <t>BUSINESS_PARCEL_BULK</t>
+  </si>
+  <si>
+    <t>SE, FI</t>
+  </si>
+  <si>
+    <t>Express Nordic 09:00</t>
+  </si>
+  <si>
+    <t>0335</t>
+  </si>
+  <si>
+    <t>EXPRESS_NORDIC_0900</t>
+  </si>
+  <si>
     <t>SE</t>
   </si>
   <si>
-    <t>Home Delivery Parcel</t>
-  </si>
-  <si>
-    <t>0349</t>
-  </si>
-  <si>
-    <t>HOME_DELIVERY_PARCEL</t>
-  </si>
-  <si>
-    <t>NO, SE, DK</t>
-  </si>
-  <si>
-    <t>Business Parcel</t>
-  </si>
-  <si>
-    <t>0330</t>
-  </si>
-  <si>
-    <t>BUSINESS_PARCEL</t>
-  </si>
-  <si>
-    <t>SE, DK, FI</t>
-  </si>
-  <si>
-    <t>Business Parcel Bulk</t>
-  </si>
-  <si>
-    <t>0332</t>
-  </si>
-  <si>
-    <t>BUSINESS_PARCEL_BULK</t>
-  </si>
-  <si>
-    <t>SE, FI</t>
-  </si>
-  <si>
-    <t>Express Nordic 09:00</t>
-  </si>
-  <si>
-    <t>0335</t>
-  </si>
-  <si>
-    <t>EXPRESS_NORDIC_0900</t>
-  </si>
-  <si>
     <t>Express Nordic 09:00 Bulk</t>
   </si>
   <si>
@@ -574,12 +566,15 @@
     <t>Supply Base Logistics</t>
   </si>
   <si>
-    <t>Oil Express</t>
-  </si>
-  <si>
     <t>OIL_EXPRESS</t>
   </si>
   <si>
+    <t>Project Logistics</t>
+  </si>
+  <si>
+    <t>PROJECT_LOGISTICS</t>
+  </si>
+  <si>
     <t>Mail</t>
   </si>
   <si>
@@ -595,7 +590,16 @@
     <t>3630</t>
   </si>
   <si>
-    <t>SE, DK, FI, AT, BE, CH, CZ, DE, EE, FR, GB, HR, HU, IE, IS, LT, LU, LV, NL, PL, SI, SK</t>
+    <t>SE, DK, FI, AT, BE, CH, CZ, DE, EE, FR, GB, HR, HU, IE, IS, IT, LT, LU, LV, NL, PL, SI, SK</t>
+  </si>
+  <si>
+    <t>Letter Packet</t>
+  </si>
+  <si>
+    <t>3639</t>
+  </si>
+  <si>
+    <t>ALL COUNTRIES EXCEPT(NO, AF, BT, IL, LY, SS, SD, SY, YE)</t>
   </si>
   <si>
     <t>* Only supported in Shipping Guide API</t>
@@ -608,34 +612,25 @@
   </si>
   <si>
     <t xml:space="preserve">Information applies to revised services only. </t>
-  </si>
-  <si>
-    <t>Letter Packet</t>
-  </si>
-  <si>
-    <t>3639</t>
-  </si>
-  <si>
-    <t>SE, DK, FI, AD, AE, AG, AI, AL, AM, AN, AO, AQ, AR, AS, AT, AU, AW, AX, AZ, BA, BB, BD, BE, BF, BG, BH, BI, BJ, BL, BM, BN, BO, BQ, BR, BS, BV, BW, BY, BZ, CA, CC, CD, CF, CG, CH, CI, CK, CL, CM, CN, CO, CR, CU, CV, CW, CX, CY, CZ, DE, DJ, DM, DO, DZ, EC, EE, EG, EH, ER, ES, ET, FJ, FK, FM, FO, FR, GA, GB, GD, GE, GF, GG, GH, GI, GL, GM, GN, GP, GQ, GR, GS, GT, GU, GW, GY, HK, HM, HN, HR, HT, HU, ID, IE, IM, IN, IO, IQ, IR, IS, IT, JE, JM, JO, JP, KE, KG, KH, KI, KM, KN, KP, KR, KW, KY, KZ, LA, LB, LC, LI, LK, LR, LS, LT, LU, LV, MA, MC, MD, ME, MF, MG, MH, MK, ML, MM, MN, MO, MP, MQ, MR, MS, MT, MU, MV, MW, MX, MY, MZ, NA, NC, NE, NF, NG, NI, NL, NP, NR, NU, NZ, OM, PA, PE, PF, PG, PH, PK, PL, PM, PN, PR, PS, PT, PW, PY, QA, RE, RO, RS, RU, RW, SA, SB, SC, SG, SH, SI, SJ, SK, SL, SM, SN, SO, SR, ST, SV, SX, SZ, TC, TD, TF, TG, TH, TJ, TK, TL, TM, TN, TO, TR, TT, TV, TW, TZ, UA, UG, UM, US, UY, UZ, VA, VC, VE, VG, VI, VN, VU, WF, WS, XK, YT, ZA, ZM, ZW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="12.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -643,16 +638,96 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="darkGray"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
+      <left>
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left>
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left>
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom>
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom>
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -667,7 +742,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -675,349 +749,41 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P56" sqref="P56"/>
+    <sheetView workbookViewId="0" tabSelected="true">
+      <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="57.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="86" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.79296875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="22.33984375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="30.23046875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.08984375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="30.46484375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="10.62109375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="7.859375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="8.265625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="15.1875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="14.5546875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="9.27734375" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="15.76953125" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="9.73828125" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="18.35546875" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="16.00390625" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="86.03515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1070,7 +836,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1123,7 +889,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -1176,7 +942,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -1229,7 +995,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1282,7 +1048,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1335,7 +1101,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1388,7 +1154,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -1441,7 +1207,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -1494,7 +1260,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1547,7 +1313,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -1600,7 +1366,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -1653,7 +1419,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -1706,7 +1472,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1756,24 +1522,24 @@
         <v>61</v>
       </c>
       <c r="Q14" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>21</v>
@@ -1800,7 +1566,7 @@
         <v>23</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>60</v>
@@ -1812,7 +1578,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1820,13 +1586,13 @@
         <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>34</v>
@@ -1853,7 +1619,7 @@
         <v>23</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>54</v>
@@ -1862,24 +1628,24 @@
         <v>55</v>
       </c>
       <c r="Q16" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>34</v>
@@ -1915,24 +1681,24 @@
         <v>61</v>
       </c>
       <c r="Q17" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>34</v>
@@ -1968,10 +1734,10 @@
         <v>22</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -2024,7 +1790,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -2074,10 +1840,10 @@
         <v>85</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -2127,10 +1893,10 @@
         <v>54</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -2177,13 +1943,13 @@
         <v>60</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -2236,7 +2002,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -2289,7 +2055,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -2342,7 +2108,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -2395,7 +2161,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="A27" s="1" t="s">
         <v>103</v>
       </c>
@@ -2448,7 +2214,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -2501,7 +2267,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -2554,7 +2320,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -2607,7 +2373,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -2660,7 +2426,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="A32" s="1" t="s">
         <v>115</v>
       </c>
@@ -2704,16 +2470,16 @@
         <v>24</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33">
       <c r="A33" s="1" t="s">
         <v>25</v>
       </c>
@@ -2757,16 +2523,16 @@
         <v>24</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
@@ -2810,16 +2576,16 @@
         <v>24</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35">
       <c r="A35" s="1" t="s">
         <v>25</v>
       </c>
@@ -2863,16 +2629,16 @@
         <v>22</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36">
       <c r="A36" s="1" t="s">
         <v>25</v>
       </c>
@@ -2925,7 +2691,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="37">
       <c r="A37" s="1" t="s">
         <v>25</v>
       </c>
@@ -2969,16 +2735,16 @@
         <v>22</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38">
       <c r="A38" s="1" t="s">
         <v>25</v>
       </c>
@@ -3022,16 +2788,16 @@
         <v>22</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39">
       <c r="A39" s="1" t="s">
         <v>25</v>
       </c>
@@ -3075,16 +2841,16 @@
         <v>22</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40">
       <c r="A40" s="1" t="s">
         <v>139</v>
       </c>
@@ -3137,7 +2903,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="41">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
@@ -3190,7 +2956,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="42">
       <c r="A42" s="1" t="s">
         <v>25</v>
       </c>
@@ -3243,7 +3009,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="43">
       <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
@@ -3296,7 +3062,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="44">
       <c r="A44" s="1" t="s">
         <v>25</v>
       </c>
@@ -3349,7 +3115,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="45">
       <c r="A45" s="1" t="s">
         <v>25</v>
       </c>
@@ -3399,10 +3165,10 @@
         <v>22</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46">
       <c r="A46" s="1" t="s">
         <v>25</v>
       </c>
@@ -3452,10 +3218,10 @@
         <v>22</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -3505,10 +3271,10 @@
         <v>22</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48">
       <c r="A48" s="1" t="s">
         <v>25</v>
       </c>
@@ -3558,10 +3324,10 @@
         <v>22</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49">
       <c r="A49" s="1" t="s">
         <v>25</v>
       </c>
@@ -3611,10 +3377,10 @@
         <v>22</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50">
       <c r="A50" s="1" t="s">
         <v>25</v>
       </c>
@@ -3667,7 +3433,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="51">
       <c r="A51" s="1" t="s">
         <v>25</v>
       </c>
@@ -3711,16 +3477,16 @@
         <v>22</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P51" s="1" t="s">
         <v>54</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52">
       <c r="A52" s="1" t="s">
         <v>176</v>
       </c>
@@ -3773,7 +3539,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="53">
       <c r="A53" s="1" t="s">
         <v>181</v>
       </c>
@@ -3781,13 +3547,13 @@
         <v>182</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>178</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>34</v>
@@ -3826,74 +3592,74 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="54">
       <c r="A54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D54" s="1" t="s">
+      <c r="F54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O54" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P54" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q54" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="B55" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F54" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J54" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L54" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M54" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N54" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O54" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P54" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q54" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C55" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>143</v>
@@ -3902,7 +3668,7 @@
         <v>22</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>22</v>
@@ -3917,36 +3683,36 @@
         <v>22</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N55" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q55" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P55" s="1" t="s">
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="Q55" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="E56" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>143</v>
@@ -3979,34 +3745,87 @@
         <v>24</v>
       </c>
       <c r="P56" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q56" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O57" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q57" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="1">
         <v>197</v>
       </c>
-      <c r="Q56" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>194</v>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="1">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P61" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <autoFilter ref="A1:P62"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dev-site, mybring-service-country-vas-common lib sync-up (#1797)
* Show Project logistics in dev-site

* Add tracking vas and show project_logistics in Ønsket leveringstid, Dangerous goods, Express vases

* Generated from latest Common-vas
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -1,29 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a2344567/projects/bring/developer-site/static/services/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2591A094-3BEE-F74D-B16F-8AD2591778AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Booking &amp; SG API" sheetId="1" r:id="rId1"/>
+    <sheet name="Booking &amp; SG API" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Booking &amp; SG API'!$A$1:$P$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$62</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="199">
   <si>
     <t>Service family</t>
   </si>
@@ -211,54 +203,54 @@
     <t>NO, SE, DK, FI, DE, EE, FO, GB, IS, NL</t>
   </si>
   <si>
+    <t>Home Delivery Parcel</t>
+  </si>
+  <si>
+    <t>0349</t>
+  </si>
+  <si>
+    <t>HOME_DELIVERY_PARCEL</t>
+  </si>
+  <si>
+    <t>NO, SE, DK</t>
+  </si>
+  <si>
+    <t>Business Parcel</t>
+  </si>
+  <si>
+    <t>0330</t>
+  </si>
+  <si>
+    <t>BUSINESS_PARCEL</t>
+  </si>
+  <si>
+    <t>SE, DK, FI</t>
+  </si>
+  <si>
+    <t>Business Parcel Bulk</t>
+  </si>
+  <si>
+    <t>0332</t>
+  </si>
+  <si>
+    <t>BUSINESS_PARCEL_BULK</t>
+  </si>
+  <si>
+    <t>SE, FI</t>
+  </si>
+  <si>
+    <t>Express Nordic 09:00</t>
+  </si>
+  <si>
+    <t>0335</t>
+  </si>
+  <si>
+    <t>EXPRESS_NORDIC_0900</t>
+  </si>
+  <si>
     <t>SE</t>
   </si>
   <si>
-    <t>Home Delivery Parcel</t>
-  </si>
-  <si>
-    <t>0349</t>
-  </si>
-  <si>
-    <t>HOME_DELIVERY_PARCEL</t>
-  </si>
-  <si>
-    <t>NO, SE, DK</t>
-  </si>
-  <si>
-    <t>Business Parcel</t>
-  </si>
-  <si>
-    <t>0330</t>
-  </si>
-  <si>
-    <t>BUSINESS_PARCEL</t>
-  </si>
-  <si>
-    <t>SE, DK, FI</t>
-  </si>
-  <si>
-    <t>Business Parcel Bulk</t>
-  </si>
-  <si>
-    <t>0332</t>
-  </si>
-  <si>
-    <t>BUSINESS_PARCEL_BULK</t>
-  </si>
-  <si>
-    <t>SE, FI</t>
-  </si>
-  <si>
-    <t>Express Nordic 09:00</t>
-  </si>
-  <si>
-    <t>0335</t>
-  </si>
-  <si>
-    <t>EXPRESS_NORDIC_0900</t>
-  </si>
-  <si>
     <t>Express Nordic 09:00 Bulk</t>
   </si>
   <si>
@@ -574,12 +566,15 @@
     <t>Supply Base Logistics</t>
   </si>
   <si>
-    <t>Oil Express</t>
-  </si>
-  <si>
     <t>OIL_EXPRESS</t>
   </si>
   <si>
+    <t>Project Logistics</t>
+  </si>
+  <si>
+    <t>PROJECT_LOGISTICS</t>
+  </si>
+  <si>
     <t>Mail</t>
   </si>
   <si>
@@ -595,7 +590,16 @@
     <t>3630</t>
   </si>
   <si>
-    <t>SE, DK, FI, AT, BE, CH, CZ, DE, EE, FR, GB, HR, HU, IE, IS, LT, LU, LV, NL, PL, SI, SK</t>
+    <t>SE, DK, FI, AT, BE, CH, CZ, DE, EE, FR, GB, HR, HU, IE, IS, IT, LT, LU, LV, NL, PL, SI, SK</t>
+  </si>
+  <si>
+    <t>Letter Packet</t>
+  </si>
+  <si>
+    <t>3639</t>
+  </si>
+  <si>
+    <t>ALL COUNTRIES EXCEPT(NO, AF, BT, IL, LY, SS, SD, SY, YE)</t>
   </si>
   <si>
     <t>* Only supported in Shipping Guide API</t>
@@ -608,34 +612,25 @@
   </si>
   <si>
     <t xml:space="preserve">Information applies to revised services only. </t>
-  </si>
-  <si>
-    <t>Letter Packet</t>
-  </si>
-  <si>
-    <t>3639</t>
-  </si>
-  <si>
-    <t>SE, DK, FI, AD, AE, AG, AI, AL, AM, AN, AO, AQ, AR, AS, AT, AU, AW, AX, AZ, BA, BB, BD, BE, BF, BG, BH, BI, BJ, BL, BM, BN, BO, BQ, BR, BS, BV, BW, BY, BZ, CA, CC, CD, CF, CG, CH, CI, CK, CL, CM, CN, CO, CR, CU, CV, CW, CX, CY, CZ, DE, DJ, DM, DO, DZ, EC, EE, EG, EH, ER, ES, ET, FJ, FK, FM, FO, FR, GA, GB, GD, GE, GF, GG, GH, GI, GL, GM, GN, GP, GQ, GR, GS, GT, GU, GW, GY, HK, HM, HN, HR, HT, HU, ID, IE, IM, IN, IO, IQ, IR, IS, IT, JE, JM, JO, JP, KE, KG, KH, KI, KM, KN, KP, KR, KW, KY, KZ, LA, LB, LC, LI, LK, LR, LS, LT, LU, LV, MA, MC, MD, ME, MF, MG, MH, MK, ML, MM, MN, MO, MP, MQ, MR, MS, MT, MU, MV, MW, MX, MY, MZ, NA, NC, NE, NF, NG, NI, NL, NP, NR, NU, NZ, OM, PA, PE, PF, PG, PH, PK, PL, PM, PN, PR, PS, PT, PW, PY, QA, RE, RO, RS, RU, RW, SA, SB, SC, SG, SH, SI, SJ, SK, SL, SM, SN, SO, SR, ST, SV, SX, SZ, TC, TD, TF, TG, TH, TJ, TK, TL, TM, TN, TO, TR, TT, TV, TW, TZ, UA, UG, UM, US, UY, UZ, VA, VC, VE, VG, VI, VN, VU, WF, WS, XK, YT, ZA, ZM, ZW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="12.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -643,16 +638,96 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="darkGray"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
+      <left>
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left>
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left>
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom>
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom>
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -667,7 +742,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -675,349 +749,41 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P56" sqref="P56"/>
+    <sheetView workbookViewId="0" tabSelected="true">
+      <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="57.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="86" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.79296875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="22.33984375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="30.23046875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.08984375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="30.46484375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="10.62109375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="7.859375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="8.265625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="15.1875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="14.5546875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="9.27734375" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="15.76953125" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="9.73828125" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="18.35546875" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="16.00390625" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="86.03515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1070,7 +836,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1123,7 +889,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -1176,7 +942,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -1229,7 +995,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1282,7 +1048,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1335,7 +1101,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1388,7 +1154,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -1441,7 +1207,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -1494,7 +1260,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1547,7 +1313,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -1600,7 +1366,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -1653,7 +1419,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -1706,7 +1472,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1756,24 +1522,24 @@
         <v>61</v>
       </c>
       <c r="Q14" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>21</v>
@@ -1800,7 +1566,7 @@
         <v>23</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>60</v>
@@ -1812,7 +1578,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1820,13 +1586,13 @@
         <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>34</v>
@@ -1853,7 +1619,7 @@
         <v>23</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>54</v>
@@ -1862,24 +1628,24 @@
         <v>55</v>
       </c>
       <c r="Q16" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>34</v>
@@ -1915,24 +1681,24 @@
         <v>61</v>
       </c>
       <c r="Q17" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>34</v>
@@ -1968,10 +1734,10 @@
         <v>22</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -2024,7 +1790,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -2074,10 +1840,10 @@
         <v>85</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -2127,10 +1893,10 @@
         <v>54</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -2177,13 +1943,13 @@
         <v>60</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -2236,7 +2002,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -2289,7 +2055,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -2342,7 +2108,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -2395,7 +2161,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="A27" s="1" t="s">
         <v>103</v>
       </c>
@@ -2448,7 +2214,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -2501,7 +2267,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -2554,7 +2320,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -2607,7 +2373,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -2660,7 +2426,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="A32" s="1" t="s">
         <v>115</v>
       </c>
@@ -2704,16 +2470,16 @@
         <v>24</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33">
       <c r="A33" s="1" t="s">
         <v>25</v>
       </c>
@@ -2757,16 +2523,16 @@
         <v>24</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
@@ -2810,16 +2576,16 @@
         <v>24</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35">
       <c r="A35" s="1" t="s">
         <v>25</v>
       </c>
@@ -2863,16 +2629,16 @@
         <v>22</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36">
       <c r="A36" s="1" t="s">
         <v>25</v>
       </c>
@@ -2925,7 +2691,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="37">
       <c r="A37" s="1" t="s">
         <v>25</v>
       </c>
@@ -2969,16 +2735,16 @@
         <v>22</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38">
       <c r="A38" s="1" t="s">
         <v>25</v>
       </c>
@@ -3022,16 +2788,16 @@
         <v>22</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39">
       <c r="A39" s="1" t="s">
         <v>25</v>
       </c>
@@ -3075,16 +2841,16 @@
         <v>22</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40">
       <c r="A40" s="1" t="s">
         <v>139</v>
       </c>
@@ -3137,7 +2903,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="41">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
@@ -3190,7 +2956,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="42">
       <c r="A42" s="1" t="s">
         <v>25</v>
       </c>
@@ -3243,7 +3009,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="43">
       <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
@@ -3296,7 +3062,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="44">
       <c r="A44" s="1" t="s">
         <v>25</v>
       </c>
@@ -3349,7 +3115,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="45">
       <c r="A45" s="1" t="s">
         <v>25</v>
       </c>
@@ -3399,10 +3165,10 @@
         <v>22</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46">
       <c r="A46" s="1" t="s">
         <v>25</v>
       </c>
@@ -3452,10 +3218,10 @@
         <v>22</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -3505,10 +3271,10 @@
         <v>22</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48">
       <c r="A48" s="1" t="s">
         <v>25</v>
       </c>
@@ -3558,10 +3324,10 @@
         <v>22</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49">
       <c r="A49" s="1" t="s">
         <v>25</v>
       </c>
@@ -3611,10 +3377,10 @@
         <v>22</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50">
       <c r="A50" s="1" t="s">
         <v>25</v>
       </c>
@@ -3667,7 +3433,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="51">
       <c r="A51" s="1" t="s">
         <v>25</v>
       </c>
@@ -3711,16 +3477,16 @@
         <v>22</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P51" s="1" t="s">
         <v>54</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52">
       <c r="A52" s="1" t="s">
         <v>176</v>
       </c>
@@ -3773,7 +3539,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="53">
       <c r="A53" s="1" t="s">
         <v>181</v>
       </c>
@@ -3781,13 +3547,13 @@
         <v>182</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>178</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>34</v>
@@ -3826,74 +3592,74 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="54">
       <c r="A54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D54" s="1" t="s">
+      <c r="F54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O54" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P54" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q54" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="B55" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F54" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J54" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L54" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M54" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N54" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O54" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P54" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q54" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C55" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>143</v>
@@ -3902,7 +3668,7 @@
         <v>22</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>22</v>
@@ -3917,36 +3683,36 @@
         <v>22</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N55" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q55" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P55" s="1" t="s">
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="Q55" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="E56" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>143</v>
@@ -3979,34 +3745,87 @@
         <v>24</v>
       </c>
       <c r="P56" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q56" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O57" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q57" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="1">
         <v>197</v>
       </c>
-      <c r="Q56" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>194</v>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="1">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P61" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <autoFilter ref="A1:P62"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update data from common library
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Booking &amp; SG API" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$63</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="201">
   <si>
     <t>Service family</t>
   </si>
@@ -236,9 +236,6 @@
     <t>BUSINESS_PARCEL_BULK</t>
   </si>
   <si>
-    <t>SE, FI</t>
-  </si>
-  <si>
     <t>Express Nordic 09:00</t>
   </si>
   <si>
@@ -326,6 +323,18 @@
     <t>BUSINESS_PARCEL_RETURN_BULK</t>
   </si>
   <si>
+    <t>Bring Pack</t>
+  </si>
+  <si>
+    <t>0360</t>
+  </si>
+  <si>
+    <t>C2C</t>
+  </si>
+  <si>
+    <t>Customer setup</t>
+  </si>
+  <si>
     <t>Cargo Norway domestic</t>
   </si>
   <si>
@@ -339,9 +348,6 @@
   </si>
   <si>
     <t>5400</t>
-  </si>
-  <si>
-    <t>Customer setup</t>
   </si>
   <si>
     <t>Business before 07:00</t>
@@ -756,7 +762,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Q61"/>
+  <dimension ref="A1:Q62"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -1681,7 +1687,7 @@
         <v>61</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18">
@@ -1692,13 +1698,13 @@
         <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>34</v>
@@ -1734,7 +1740,7 @@
         <v>22</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19">
@@ -1745,13 +1751,13 @@
         <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>34</v>
@@ -1784,7 +1790,7 @@
         <v>60</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>22</v>
@@ -1798,13 +1804,13 @@
         <v>25</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>34</v>
@@ -1837,7 +1843,7 @@
         <v>60</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>69</v>
@@ -1851,13 +1857,13 @@
         <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>34</v>
@@ -1904,13 +1910,13 @@
         <v>25</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>34</v>
@@ -1957,13 +1963,13 @@
         <v>25</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>39</v>
@@ -1975,7 +1981,7 @@
         <v>23</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>23</v>
@@ -2010,13 +2016,13 @@
         <v>25</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>39</v>
@@ -2028,7 +2034,7 @@
         <v>23</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>23</v>
@@ -2063,13 +2069,13 @@
         <v>25</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>46</v>
@@ -2081,7 +2087,7 @@
         <v>23</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>23</v>
@@ -2116,13 +2122,13 @@
         <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>46</v>
@@ -2134,7 +2140,7 @@
         <v>23</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>23</v>
@@ -2163,32 +2169,32 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="E27" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="G27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="J27" s="1" t="s">
         <v>23</v>
       </c>
@@ -2202,33 +2208,33 @@
         <v>23</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>34</v>
@@ -2240,7 +2246,7 @@
         <v>23</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>108</v>
+        <v>22</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>23</v>
@@ -2293,7 +2299,7 @@
         <v>23</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>23</v>
@@ -2308,7 +2314,7 @@
         <v>23</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>22</v>
@@ -2390,10 +2396,10 @@
         <v>114</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>23</v>
@@ -2428,72 +2434,72 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="E32" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>108</v>
+        <v>22</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M32" s="1" t="s">
         <v>23</v>
       </c>
       <c r="N32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q32" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="O32" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q32" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>25</v>
+        <v>117</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>21</v>
@@ -2502,10 +2508,10 @@
         <v>22</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>23</v>
@@ -2540,13 +2546,13 @@
         <v>25</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>21</v>
@@ -2558,7 +2564,7 @@
         <v>23</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>23</v>
@@ -2593,13 +2599,13 @@
         <v>25</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>21</v>
@@ -2611,7 +2617,7 @@
         <v>23</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>23</v>
@@ -2626,7 +2632,7 @@
         <v>23</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O35" s="1" t="s">
         <v>65</v>
@@ -2646,10 +2652,10 @@
         <v>25</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>129</v>
@@ -2664,7 +2670,7 @@
         <v>23</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>23</v>
@@ -2682,13 +2688,13 @@
         <v>22</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37">
@@ -2705,19 +2711,19 @@
         <v>131</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>23</v>
@@ -2735,13 +2741,13 @@
         <v>22</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38">
@@ -2752,13 +2758,13 @@
         <v>25</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>39</v>
@@ -2770,7 +2776,7 @@
         <v>23</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>23</v>
@@ -2805,13 +2811,13 @@
         <v>25</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>39</v>
@@ -2823,7 +2829,7 @@
         <v>23</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>23</v>
@@ -2852,40 +2858,40 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="F40" s="1" t="s">
-        <v>143</v>
+        <v>39</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M40" s="1" t="s">
         <v>23</v>
@@ -2894,33 +2900,33 @@
         <v>22</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>25</v>
+        <v>141</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>25</v>
+        <v>141</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>22</v>
@@ -2964,16 +2970,16 @@
         <v>25</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="F42" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>22</v>
@@ -3017,16 +3023,16 @@
         <v>25</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="F43" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>22</v>
@@ -3070,16 +3076,16 @@
         <v>25</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="F44" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>22</v>
@@ -3123,16 +3129,16 @@
         <v>25</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="F45" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>22</v>
@@ -3165,7 +3171,7 @@
         <v>22</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46">
@@ -3176,16 +3182,16 @@
         <v>25</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="F46" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>22</v>
@@ -3229,16 +3235,16 @@
         <v>25</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="F47" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>22</v>
@@ -3282,16 +3288,16 @@
         <v>25</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="F48" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>22</v>
@@ -3335,16 +3341,16 @@
         <v>25</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="F49" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>22</v>
@@ -3388,16 +3394,16 @@
         <v>25</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>172</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>22</v>
@@ -3406,7 +3412,7 @@
         <v>23</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>108</v>
+        <v>22</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>23</v>
@@ -3415,10 +3421,10 @@
         <v>23</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N50" s="1" t="s">
         <v>22</v>
@@ -3430,7 +3436,7 @@
         <v>22</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51">
@@ -3444,13 +3450,13 @@
         <v>173</v>
       </c>
       <c r="D51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="F51" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>22</v>
@@ -3459,7 +3465,7 @@
         <v>23</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>23</v>
@@ -3471,39 +3477,39 @@
         <v>22</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N51" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="P51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q51" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="Q51" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C52" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="F52" s="1" t="s">
-        <v>34</v>
+        <v>145</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>22</v>
@@ -3521,39 +3527,39 @@
         <v>23</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N52" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>180</v>
+        <v>65</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>180</v>
+        <v>54</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>34</v>
@@ -3571,39 +3577,39 @@
         <v>23</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N53" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>22</v>
+        <v>182</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>22</v>
+        <v>182</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>25</v>
+        <v>183</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>25</v>
+        <v>184</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>184</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>185</v>
@@ -3618,7 +3624,7 @@
         <v>23</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>108</v>
+        <v>22</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>23</v>
@@ -3636,18 +3642,18 @@
         <v>22</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>186</v>
+        <v>25</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>25</v>
@@ -3656,28 +3662,28 @@
         <v>186</v>
       </c>
       <c r="D55" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="F55" s="1" t="s">
-        <v>143</v>
+        <v>34</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L55" s="1" t="s">
         <v>22</v>
@@ -3689,39 +3695,39 @@
         <v>22</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>25</v>
+        <v>188</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>190</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>22</v>
@@ -3736,19 +3742,19 @@
         <v>22</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N56" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q56" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="P56" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q56" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="57">
@@ -3759,16 +3765,16 @@
         <v>25</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="E57" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>22</v>
@@ -3798,34 +3804,87 @@
         <v>24</v>
       </c>
       <c r="P57" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q57" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="Q57" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s" s="0">
+      <c r="D58" s="1" t="s">
         <v>195</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P58" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q58" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="s" s="1">
-        <v>197</v>
+      <c r="A60" t="s" s="0">
+        <v>198</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="1">
-        <v>198</v>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="1">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P62"/>
+  <autoFilter ref="A1:P63"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All HD/courier services can be requested on CMN
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -122,7 +122,7 @@
     <t>B2B</t>
   </si>
   <si>
-    <t>Express next day</t>
+    <t>Business parcel express</t>
   </si>
   <si>
     <t>4850</t>
@@ -772,7 +772,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="57.79296875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="22.33984375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="21.63671875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="30.23046875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.08984375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="30.46484375" customWidth="true" bestFit="true"/>
@@ -2490,7 +2490,7 @@
         <v>117</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>118</v>
@@ -2914,7 +2914,7 @@
         <v>141</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>141</v>
+        <v>18</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>142</v>

</xml_diff>

<commit_message>
Removing Slovenia and Switzerland as supported countries for 0336 Business pallet
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -95,19 +95,19 @@
     <t/>
   </si>
   <si>
-    <t>Home delivery parcel</t>
+    <t>Parcel home plus</t>
   </si>
   <si>
     <t>5600</t>
   </si>
   <si>
-    <t>Mailbox parcel</t>
+    <t>Home mailbox parcel</t>
   </si>
   <si>
     <t>3584</t>
   </si>
   <si>
-    <t>Mailbox parcel with RFID</t>
+    <t>Home mailbox parcel RFID</t>
   </si>
   <si>
     <t>3570</t>
@@ -269,7 +269,7 @@
     <t>BUSINESS_PALLET</t>
   </si>
   <si>
-    <t>NO, SE, DK, FI, AT, AX, BE, CH, CZ, DE, EE, ES, FO, FR, GL, GR, HU, IE, IS, IT, LT, LU, LV, NL, PL, PT, SI</t>
+    <t>NO, SE, DK, FI, AT, AX, BE, CZ, DE, EE, ES, FO, FR, GL, GR, HU, IE, IS, IT, LT, LU, LV, NL, PL, PT</t>
   </si>
   <si>
     <t>Business Pallet (1/2 pallet)</t>
@@ -786,7 +786,7 @@
     <col min="13" max="13" width="9.73828125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="18.35546875" customWidth="true" bestFit="true"/>
     <col min="15" max="15" width="16.00390625" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="86.03515625" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="79.9140625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Update common lib data
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="202">
   <si>
     <t>Service family</t>
   </si>
@@ -594,6 +594,9 @@
   </si>
   <si>
     <t>3630</t>
+  </si>
+  <si>
+    <t>B2X_L</t>
   </si>
   <si>
     <t>SE, DK, FI, AT, BE, CH, CZ, DE, EE, FR, GB, HR, HU, IE, IS, IT, LT, LU, LV, NL, PL, SI, SK</t>
@@ -2211,10 +2214,10 @@
         <v>22</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="Q27" s="1" t="s">
         <v>53</v>
@@ -3774,7 +3777,7 @@
         <v>192</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>145</v>
+        <v>193</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>22</v>
@@ -3804,7 +3807,7 @@
         <v>24</v>
       </c>
       <c r="P57" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="Q57" s="1" t="s">
         <v>22</v>
@@ -3818,16 +3821,16 @@
         <v>25</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>145</v>
+        <v>193</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>22</v>
@@ -3857,7 +3860,7 @@
         <v>24</v>
       </c>
       <c r="P58" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="Q58" s="1" t="s">
         <v>22</v>
@@ -3865,22 +3868,22 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="1">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="1">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove 0344, 3630, and FI for 0360
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Booking &amp; SG API" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$62</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="199">
   <si>
     <t>Service family</t>
   </si>
@@ -590,22 +590,13 @@
     <t>MAIL*</t>
   </si>
   <si>
-    <t>International Tracked Packet</t>
-  </si>
-  <si>
-    <t>3630</t>
+    <t>Letter Packet</t>
+  </si>
+  <si>
+    <t>3639</t>
   </si>
   <si>
     <t>B2X_L</t>
-  </si>
-  <si>
-    <t>SE, DK, FI, AT, BE, CH, CZ, DE, EE, FR, GB, HR, HU, IE, IS, IT, LT, LU, LV, NL, PL, SI, SK</t>
-  </si>
-  <si>
-    <t>Letter Packet</t>
-  </si>
-  <si>
-    <t>3639</t>
   </si>
   <si>
     <t>ALL COUNTRIES EXCEPT(NO, AF, BT, IL, LY, SS, SD, SY, YE)</t>
@@ -765,7 +756,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Q62"/>
+  <dimension ref="A1:Q61"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -2214,10 +2205,10 @@
         <v>22</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="Q27" s="1" t="s">
         <v>53</v>
@@ -3814,80 +3805,27 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C58" s="1" t="s">
+      <c r="A58" t="s" s="0">
         <v>195</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J58" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K58" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O58" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P58" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="Q58" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="s" s="0">
-        <v>199</v>
+      <c r="A60" t="s" s="1">
+        <v>197</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s" s="1">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P63"/>
+  <autoFilter ref="A1:P62"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hide 3336 in service portfolio
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Booking &amp; SG API" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$61</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="196">
   <si>
     <t>Service family</t>
   </si>
@@ -540,15 +540,6 @@
   </si>
   <si>
     <t>NON_STANDARD_COURIER</t>
-  </si>
-  <si>
-    <t>Express Same Day</t>
-  </si>
-  <si>
-    <t>3336</t>
-  </si>
-  <si>
-    <t>EXPRESS_NORDIC_SAME_DAY</t>
   </si>
   <si>
     <t>Cargo Norway international</t>
@@ -756,7 +747,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Q61"/>
+  <dimension ref="A1:Q60"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -3488,22 +3479,22 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>25</v>
+        <v>175</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>145</v>
+        <v>34</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>22</v>
@@ -3521,39 +3512,39 @@
         <v>23</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N52" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>65</v>
+        <v>179</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>54</v>
+        <v>179</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>18</v>
+        <v>181</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>34</v>
@@ -3571,42 +3562,42 @@
         <v>23</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N53" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>182</v>
+        <v>22</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>182</v>
+        <v>22</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="D54" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>34</v>
@@ -3618,7 +3609,7 @@
         <v>23</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>23</v>
@@ -3636,48 +3627,48 @@
         <v>22</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>187</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>34</v>
+        <v>145</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L55" s="1" t="s">
         <v>22</v>
@@ -3689,18 +3680,18 @@
         <v>22</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>188</v>
+        <v>25</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>25</v>
@@ -3712,16 +3703,16 @@
         <v>189</v>
       </c>
       <c r="E56" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="F56" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="G56" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>22</v>
@@ -3736,96 +3727,43 @@
         <v>22</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N56" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>22</v>
+        <v>191</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D57" s="1" t="s">
+      <c r="A57" t="s" s="0">
         <v>192</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J57" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K57" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O57" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P57" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q57" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="s" s="0">
-        <v>196</v>
+      <c r="A59" t="s" s="1">
+        <v>194</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="1">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="s" s="1">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P62"/>
+  <autoFilter ref="A1:P61"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add revised courier and distribution services in dev site replacing old courier services in booking-api
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Booking &amp; SG API" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$66</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="197">
   <si>
     <t>Service family</t>
   </si>
@@ -443,103 +443,103 @@
     <t>Courier and Express</t>
   </si>
   <si>
-    <t>Courier 1 hour</t>
-  </si>
-  <si>
-    <t>1H25</t>
-  </si>
-  <si>
-    <t>COURIER_1H</t>
+    <t>Courier Distribution</t>
+  </si>
+  <si>
+    <t>3270</t>
   </si>
   <si>
     <t>B2X</t>
   </si>
   <si>
-    <t>Courier 2 hours</t>
-  </si>
-  <si>
-    <t>2H25</t>
-  </si>
-  <si>
-    <t>COURIER_2H</t>
-  </si>
-  <si>
-    <t>Courier 4 hours</t>
-  </si>
-  <si>
-    <t>4H25</t>
-  </si>
-  <si>
-    <t>COURIER_4H</t>
-  </si>
-  <si>
-    <t>Courier 6 hours</t>
-  </si>
-  <si>
-    <t>6H25</t>
-  </si>
-  <si>
-    <t>COURIER_6H</t>
-  </si>
-  <si>
-    <t>Courier VIP</t>
-  </si>
-  <si>
-    <t>VIP25</t>
-  </si>
-  <si>
-    <t>COURIER_VIP</t>
-  </si>
-  <si>
-    <t>Courier Long Distance</t>
-  </si>
-  <si>
-    <t>LD25</t>
-  </si>
-  <si>
-    <t>COURIER_LONG_DISTANCE</t>
-  </si>
-  <si>
-    <t>Bicycle 1 hour</t>
-  </si>
-  <si>
-    <t>B1H5</t>
-  </si>
-  <si>
-    <t>COURIER_BICYCLE_1H</t>
-  </si>
-  <si>
-    <t>Bicycle 2 hours</t>
-  </si>
-  <si>
-    <t>B2H5</t>
-  </si>
-  <si>
-    <t>COURIER_BICYCLE_2H</t>
-  </si>
-  <si>
-    <t>Bicycle 4 hours</t>
-  </si>
-  <si>
-    <t>B4H5</t>
-  </si>
-  <si>
-    <t>COURIER_BICYCLE_4H</t>
-  </si>
-  <si>
-    <t>Bicycle VIP</t>
-  </si>
-  <si>
-    <t>BVIP5</t>
-  </si>
-  <si>
-    <t>COURIER_BICYCLE_VIP</t>
-  </si>
-  <si>
-    <t>Courier Non Standard</t>
-  </si>
-  <si>
-    <t>NON_STANDARD_COURIER</t>
+    <t>Courier Distribution Pallet</t>
+  </si>
+  <si>
+    <t>3271</t>
+  </si>
+  <si>
+    <t>Long Distance Courier</t>
+  </si>
+  <si>
+    <t>3624</t>
+  </si>
+  <si>
+    <t>Premium Courier</t>
+  </si>
+  <si>
+    <t>3625</t>
+  </si>
+  <si>
+    <t>Standard Courier</t>
+  </si>
+  <si>
+    <t>3627</t>
+  </si>
+  <si>
+    <t>Economy Courier</t>
+  </si>
+  <si>
+    <t>3629</t>
+  </si>
+  <si>
+    <t>Same day distribution temp</t>
+  </si>
+  <si>
+    <t>3619</t>
+  </si>
+  <si>
+    <t>Same day distribution parcel</t>
+  </si>
+  <si>
+    <t>3620</t>
+  </si>
+  <si>
+    <t>Same day distribution pallet</t>
+  </si>
+  <si>
+    <t>3621</t>
+  </si>
+  <si>
+    <t>Long Distance Courier Truck</t>
+  </si>
+  <si>
+    <t>3654</t>
+  </si>
+  <si>
+    <t>Premium Courier Truck</t>
+  </si>
+  <si>
+    <t>3655</t>
+  </si>
+  <si>
+    <t>Standard Courier Truck</t>
+  </si>
+  <si>
+    <t>3657</t>
+  </si>
+  <si>
+    <t>Economy Courier Truck</t>
+  </si>
+  <si>
+    <t>3659</t>
+  </si>
+  <si>
+    <t>Premium Courier Bicycle</t>
+  </si>
+  <si>
+    <t>3665</t>
+  </si>
+  <si>
+    <t>Standard Courier Bicycle</t>
+  </si>
+  <si>
+    <t>3667</t>
+  </si>
+  <si>
+    <t>Economy Courier Bicycle</t>
+  </si>
+  <si>
+    <t>3669</t>
   </si>
   <si>
     <t>Cargo Norway international</t>
@@ -570,6 +570,9 @@
   </si>
   <si>
     <t>PROJECT_LOGISTICS</t>
+  </si>
+  <si>
+    <t>Letter</t>
   </si>
   <si>
     <t>Mail</t>
@@ -747,7 +750,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Q60"/>
+  <dimension ref="A1:Q65"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -2908,10 +2911,10 @@
         <v>143</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>22</v>
@@ -2955,16 +2958,16 @@
         <v>25</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="E42" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>22</v>
@@ -3008,16 +3011,16 @@
         <v>25</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>22</v>
@@ -3061,16 +3064,16 @@
         <v>25</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>22</v>
@@ -3114,16 +3117,16 @@
         <v>25</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>22</v>
@@ -3167,16 +3170,16 @@
         <v>25</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>22</v>
@@ -3209,7 +3212,7 @@
         <v>22</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47">
@@ -3220,16 +3223,16 @@
         <v>25</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>145</v>
+        <v>21</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>22</v>
@@ -3262,7 +3265,7 @@
         <v>22</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48">
@@ -3273,16 +3276,16 @@
         <v>25</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>22</v>
@@ -3315,7 +3318,7 @@
         <v>22</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49">
@@ -3326,16 +3329,16 @@
         <v>25</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>22</v>
@@ -3368,7 +3371,7 @@
         <v>22</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50">
@@ -3379,16 +3382,16 @@
         <v>25</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>22</v>
@@ -3421,7 +3424,7 @@
         <v>22</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51">
@@ -3432,16 +3435,16 @@
         <v>25</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>25</v>
+        <v>164</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>22</v>
@@ -3450,7 +3453,7 @@
         <v>23</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>23</v>
@@ -3459,10 +3462,10 @@
         <v>23</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N51" s="1" t="s">
         <v>22</v>
@@ -3479,22 +3482,22 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>175</v>
+        <v>25</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>34</v>
+        <v>144</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>22</v>
@@ -3515,39 +3518,39 @@
         <v>23</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N52" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>179</v>
+        <v>22</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>179</v>
+        <v>22</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>180</v>
+        <v>25</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>181</v>
+        <v>25</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>34</v>
+        <v>144</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>22</v>
@@ -3562,10 +3565,10 @@
         <v>23</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M53" s="1" t="s">
         <v>23</v>
@@ -3580,7 +3583,7 @@
         <v>22</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54">
@@ -3591,16 +3594,16 @@
         <v>25</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>34</v>
+        <v>144</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>22</v>
@@ -3609,16 +3612,16 @@
         <v>23</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M54" s="1" t="s">
         <v>23</v>
@@ -3627,39 +3630,39 @@
         <v>22</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>185</v>
+        <v>25</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>22</v>
@@ -3671,7 +3674,7 @@
         <v>23</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M55" s="1" t="s">
         <v>23</v>
@@ -3686,7 +3689,7 @@
         <v>22</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56">
@@ -3697,73 +3700,338 @@
         <v>25</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q56" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O57" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q57" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q58" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P59" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q59" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="F60" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q60" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="F56" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="G56" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J56" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M56" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N56" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O56" s="1" t="s">
+      <c r="E61" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O61" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P56" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q56" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s" s="0">
+      <c r="P61" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s" s="0">
+      <c r="Q61" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="0">
         <v>193</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="s" s="1">
+    <row r="63">
+      <c r="A63" t="s" s="0">
         <v>194</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" t="s" s="1">
+    <row r="64">
+      <c r="A64" t="s" s="1">
         <v>195</v>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" t="s" s="1">
+        <v>196</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:P61"/>
+  <autoFilter ref="A1:P66"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add revised courier and distribution services in dev site replacing old courier services in booking-api (#1888)
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Booking &amp; SG API" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$66</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="197">
   <si>
     <t>Service family</t>
   </si>
@@ -443,103 +443,103 @@
     <t>Courier and Express</t>
   </si>
   <si>
-    <t>Courier 1 hour</t>
-  </si>
-  <si>
-    <t>1H25</t>
-  </si>
-  <si>
-    <t>COURIER_1H</t>
+    <t>Courier Distribution</t>
+  </si>
+  <si>
+    <t>3270</t>
   </si>
   <si>
     <t>B2X</t>
   </si>
   <si>
-    <t>Courier 2 hours</t>
-  </si>
-  <si>
-    <t>2H25</t>
-  </si>
-  <si>
-    <t>COURIER_2H</t>
-  </si>
-  <si>
-    <t>Courier 4 hours</t>
-  </si>
-  <si>
-    <t>4H25</t>
-  </si>
-  <si>
-    <t>COURIER_4H</t>
-  </si>
-  <si>
-    <t>Courier 6 hours</t>
-  </si>
-  <si>
-    <t>6H25</t>
-  </si>
-  <si>
-    <t>COURIER_6H</t>
-  </si>
-  <si>
-    <t>Courier VIP</t>
-  </si>
-  <si>
-    <t>VIP25</t>
-  </si>
-  <si>
-    <t>COURIER_VIP</t>
-  </si>
-  <si>
-    <t>Courier Long Distance</t>
-  </si>
-  <si>
-    <t>LD25</t>
-  </si>
-  <si>
-    <t>COURIER_LONG_DISTANCE</t>
-  </si>
-  <si>
-    <t>Bicycle 1 hour</t>
-  </si>
-  <si>
-    <t>B1H5</t>
-  </si>
-  <si>
-    <t>COURIER_BICYCLE_1H</t>
-  </si>
-  <si>
-    <t>Bicycle 2 hours</t>
-  </si>
-  <si>
-    <t>B2H5</t>
-  </si>
-  <si>
-    <t>COURIER_BICYCLE_2H</t>
-  </si>
-  <si>
-    <t>Bicycle 4 hours</t>
-  </si>
-  <si>
-    <t>B4H5</t>
-  </si>
-  <si>
-    <t>COURIER_BICYCLE_4H</t>
-  </si>
-  <si>
-    <t>Bicycle VIP</t>
-  </si>
-  <si>
-    <t>BVIP5</t>
-  </si>
-  <si>
-    <t>COURIER_BICYCLE_VIP</t>
-  </si>
-  <si>
-    <t>Courier Non Standard</t>
-  </si>
-  <si>
-    <t>NON_STANDARD_COURIER</t>
+    <t>Courier Distribution Pallet</t>
+  </si>
+  <si>
+    <t>3271</t>
+  </si>
+  <si>
+    <t>Long Distance Courier</t>
+  </si>
+  <si>
+    <t>3624</t>
+  </si>
+  <si>
+    <t>Premium Courier</t>
+  </si>
+  <si>
+    <t>3625</t>
+  </si>
+  <si>
+    <t>Standard Courier</t>
+  </si>
+  <si>
+    <t>3627</t>
+  </si>
+  <si>
+    <t>Economy Courier</t>
+  </si>
+  <si>
+    <t>3629</t>
+  </si>
+  <si>
+    <t>Same day distribution temp</t>
+  </si>
+  <si>
+    <t>3619</t>
+  </si>
+  <si>
+    <t>Same day distribution parcel</t>
+  </si>
+  <si>
+    <t>3620</t>
+  </si>
+  <si>
+    <t>Same day distribution pallet</t>
+  </si>
+  <si>
+    <t>3621</t>
+  </si>
+  <si>
+    <t>Long Distance Courier Truck</t>
+  </si>
+  <si>
+    <t>3654</t>
+  </si>
+  <si>
+    <t>Premium Courier Truck</t>
+  </si>
+  <si>
+    <t>3655</t>
+  </si>
+  <si>
+    <t>Standard Courier Truck</t>
+  </si>
+  <si>
+    <t>3657</t>
+  </si>
+  <si>
+    <t>Economy Courier Truck</t>
+  </si>
+  <si>
+    <t>3659</t>
+  </si>
+  <si>
+    <t>Premium Courier Bicycle</t>
+  </si>
+  <si>
+    <t>3665</t>
+  </si>
+  <si>
+    <t>Standard Courier Bicycle</t>
+  </si>
+  <si>
+    <t>3667</t>
+  </si>
+  <si>
+    <t>Economy Courier Bicycle</t>
+  </si>
+  <si>
+    <t>3669</t>
   </si>
   <si>
     <t>Cargo Norway international</t>
@@ -570,6 +570,9 @@
   </si>
   <si>
     <t>PROJECT_LOGISTICS</t>
+  </si>
+  <si>
+    <t>Letter</t>
   </si>
   <si>
     <t>Mail</t>
@@ -747,7 +750,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Q60"/>
+  <dimension ref="A1:Q65"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -2908,10 +2911,10 @@
         <v>143</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>22</v>
@@ -2955,16 +2958,16 @@
         <v>25</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="E42" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>22</v>
@@ -3008,16 +3011,16 @@
         <v>25</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>22</v>
@@ -3061,16 +3064,16 @@
         <v>25</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>22</v>
@@ -3114,16 +3117,16 @@
         <v>25</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>22</v>
@@ -3167,16 +3170,16 @@
         <v>25</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>22</v>
@@ -3209,7 +3212,7 @@
         <v>22</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47">
@@ -3220,16 +3223,16 @@
         <v>25</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>145</v>
+        <v>21</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>22</v>
@@ -3262,7 +3265,7 @@
         <v>22</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48">
@@ -3273,16 +3276,16 @@
         <v>25</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>22</v>
@@ -3315,7 +3318,7 @@
         <v>22</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49">
@@ -3326,16 +3329,16 @@
         <v>25</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>22</v>
@@ -3368,7 +3371,7 @@
         <v>22</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50">
@@ -3379,16 +3382,16 @@
         <v>25</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>22</v>
@@ -3421,7 +3424,7 @@
         <v>22</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51">
@@ -3432,16 +3435,16 @@
         <v>25</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>25</v>
+        <v>164</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>22</v>
@@ -3450,7 +3453,7 @@
         <v>23</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>23</v>
@@ -3459,10 +3462,10 @@
         <v>23</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N51" s="1" t="s">
         <v>22</v>
@@ -3479,22 +3482,22 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>175</v>
+        <v>25</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>34</v>
+        <v>144</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>22</v>
@@ -3515,39 +3518,39 @@
         <v>23</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N52" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>179</v>
+        <v>22</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>179</v>
+        <v>22</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>180</v>
+        <v>25</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>181</v>
+        <v>25</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>34</v>
+        <v>144</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>22</v>
@@ -3562,10 +3565,10 @@
         <v>23</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M53" s="1" t="s">
         <v>23</v>
@@ -3580,7 +3583,7 @@
         <v>22</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54">
@@ -3591,16 +3594,16 @@
         <v>25</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>34</v>
+        <v>144</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>22</v>
@@ -3609,16 +3612,16 @@
         <v>23</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M54" s="1" t="s">
         <v>23</v>
@@ -3627,39 +3630,39 @@
         <v>22</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>185</v>
+        <v>25</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>22</v>
@@ -3671,7 +3674,7 @@
         <v>23</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M55" s="1" t="s">
         <v>23</v>
@@ -3686,7 +3689,7 @@
         <v>22</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56">
@@ -3697,73 +3700,338 @@
         <v>25</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q56" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O57" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q57" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q58" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P59" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q59" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="F60" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q60" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="F56" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="G56" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J56" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M56" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N56" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O56" s="1" t="s">
+      <c r="E61" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O61" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P56" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q56" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s" s="0">
+      <c r="P61" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s" s="0">
+      <c r="Q61" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="0">
         <v>193</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="s" s="1">
+    <row r="63">
+      <c r="A63" t="s" s="0">
         <v>194</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" t="s" s="1">
+    <row r="64">
+      <c r="A64" t="s" s="1">
         <v>195</v>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" t="s" s="1">
+        <v>196</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:P61"/>
+  <autoFilter ref="A1:P66"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update customer setup field for revised courier and distribution services
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="198">
   <si>
     <t>Service family</t>
   </si>
@@ -443,45 +443,90 @@
     <t>Courier and Express</t>
   </si>
   <si>
+    <t>Long Distance Courier</t>
+  </si>
+  <si>
+    <t>3624</t>
+  </si>
+  <si>
+    <t>B2X</t>
+  </si>
+  <si>
+    <t>Premium Courier</t>
+  </si>
+  <si>
+    <t>3625</t>
+  </si>
+  <si>
+    <t>Customer setup (in FINLAND)</t>
+  </si>
+  <si>
+    <t>Standard Courier</t>
+  </si>
+  <si>
+    <t>3627</t>
+  </si>
+  <si>
+    <t>Economy Courier</t>
+  </si>
+  <si>
+    <t>3629</t>
+  </si>
+  <si>
+    <t>Long Distance Courier Truck</t>
+  </si>
+  <si>
+    <t>3654</t>
+  </si>
+  <si>
+    <t>Premium Courier Truck</t>
+  </si>
+  <si>
+    <t>3655</t>
+  </si>
+  <si>
+    <t>Standard Courier Truck</t>
+  </si>
+  <si>
+    <t>3657</t>
+  </si>
+  <si>
+    <t>Economy Courier Truck</t>
+  </si>
+  <si>
+    <t>3659</t>
+  </si>
+  <si>
+    <t>Premium Courier Bicycle</t>
+  </si>
+  <si>
+    <t>3665</t>
+  </si>
+  <si>
+    <t>Standard Courier Bicycle</t>
+  </si>
+  <si>
+    <t>3667</t>
+  </si>
+  <si>
+    <t>Economy Courier Bicycle</t>
+  </si>
+  <si>
+    <t>3669</t>
+  </si>
+  <si>
     <t>Courier Distribution</t>
   </si>
   <si>
     <t>3270</t>
   </si>
   <si>
-    <t>B2X</t>
-  </si>
-  <si>
     <t>Courier Distribution Pallet</t>
   </si>
   <si>
     <t>3271</t>
   </si>
   <si>
-    <t>Long Distance Courier</t>
-  </si>
-  <si>
-    <t>3624</t>
-  </si>
-  <si>
-    <t>Premium Courier</t>
-  </si>
-  <si>
-    <t>3625</t>
-  </si>
-  <si>
-    <t>Standard Courier</t>
-  </si>
-  <si>
-    <t>3627</t>
-  </si>
-  <si>
-    <t>Economy Courier</t>
-  </si>
-  <si>
-    <t>3629</t>
-  </si>
-  <si>
     <t>Same day distribution temp</t>
   </si>
   <si>
@@ -498,48 +543,6 @@
   </si>
   <si>
     <t>3621</t>
-  </si>
-  <si>
-    <t>Long Distance Courier Truck</t>
-  </si>
-  <si>
-    <t>3654</t>
-  </si>
-  <si>
-    <t>Premium Courier Truck</t>
-  </si>
-  <si>
-    <t>3655</t>
-  </si>
-  <si>
-    <t>Standard Courier Truck</t>
-  </si>
-  <si>
-    <t>3657</t>
-  </si>
-  <si>
-    <t>Economy Courier Truck</t>
-  </si>
-  <si>
-    <t>3659</t>
-  </si>
-  <si>
-    <t>Premium Courier Bicycle</t>
-  </si>
-  <si>
-    <t>3665</t>
-  </si>
-  <si>
-    <t>Standard Courier Bicycle</t>
-  </si>
-  <si>
-    <t>3667</t>
-  </si>
-  <si>
-    <t>Economy Courier Bicycle</t>
-  </si>
-  <si>
-    <t>3669</t>
   </si>
   <si>
     <t>Cargo Norway international</t>
@@ -767,7 +770,7 @@
     <col min="6" max="6" width="10.62109375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="7.859375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="8.265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="15.1875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="27.15625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="14.5546875" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="9.27734375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="15.76953125" customWidth="true" bestFit="true"/>
@@ -2923,7 +2926,7 @@
         <v>23</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>23</v>
@@ -2976,7 +2979,7 @@
         <v>23</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>22</v>
+        <v>147</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>23</v>
@@ -3011,13 +3014,13 @@
         <v>25</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>144</v>
@@ -3029,7 +3032,7 @@
         <v>23</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>22</v>
+        <v>147</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>23</v>
@@ -3064,13 +3067,13 @@
         <v>25</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>144</v>
@@ -3082,7 +3085,7 @@
         <v>23</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>22</v>
+        <v>147</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>23</v>
@@ -3117,13 +3120,13 @@
         <v>25</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>144</v>
@@ -3135,7 +3138,7 @@
         <v>23</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>23</v>
@@ -3170,13 +3173,13 @@
         <v>25</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>144</v>
@@ -3188,7 +3191,7 @@
         <v>23</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>23</v>
@@ -3223,16 +3226,16 @@
         <v>25</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>21</v>
+        <v>144</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>22</v>
@@ -3241,7 +3244,7 @@
         <v>23</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>23</v>
@@ -3276,13 +3279,13 @@
         <v>25</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>144</v>
@@ -3294,7 +3297,7 @@
         <v>23</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>23</v>
@@ -3329,13 +3332,13 @@
         <v>25</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>144</v>
@@ -3347,7 +3350,7 @@
         <v>23</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>23</v>
@@ -3371,7 +3374,7 @@
         <v>22</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50">
@@ -3382,13 +3385,13 @@
         <v>25</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>144</v>
@@ -3400,7 +3403,7 @@
         <v>23</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>23</v>
@@ -3424,7 +3427,7 @@
         <v>22</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51">
@@ -3435,13 +3438,13 @@
         <v>25</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>144</v>
@@ -3453,7 +3456,7 @@
         <v>23</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>23</v>
@@ -3477,7 +3480,7 @@
         <v>22</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52">
@@ -3488,13 +3491,13 @@
         <v>25</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>144</v>
@@ -3506,7 +3509,7 @@
         <v>23</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>23</v>
@@ -3541,13 +3544,13 @@
         <v>25</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>144</v>
@@ -3559,7 +3562,7 @@
         <v>23</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>23</v>
@@ -3594,16 +3597,16 @@
         <v>25</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>144</v>
+        <v>21</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>22</v>
@@ -3612,7 +3615,7 @@
         <v>23</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>23</v>
@@ -3636,7 +3639,7 @@
         <v>22</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55">
@@ -3647,13 +3650,13 @@
         <v>25</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>144</v>
@@ -3665,7 +3668,7 @@
         <v>23</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>23</v>
@@ -3689,7 +3692,7 @@
         <v>22</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56">
@@ -3700,13 +3703,13 @@
         <v>25</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>144</v>
@@ -3718,7 +3721,7 @@
         <v>23</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>23</v>
@@ -3742,24 +3745,24 @@
         <v>22</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>34</v>
@@ -3789,10 +3792,10 @@
         <v>22</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="P57" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="Q57" s="1" t="s">
         <v>22</v>
@@ -3800,19 +3803,19 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>34</v>
@@ -3859,13 +3862,13 @@
         <v>25</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>34</v>
@@ -3906,19 +3909,19 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>144</v>
@@ -3965,16 +3968,16 @@
         <v>25</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>22</v>
@@ -4004,7 +4007,7 @@
         <v>24</v>
       </c>
       <c r="P61" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="Q61" s="1" t="s">
         <v>22</v>
@@ -4012,22 +4015,22 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="1">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="1">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update customer setup field for revised courier and distribution services (#1889)
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="198">
   <si>
     <t>Service family</t>
   </si>
@@ -443,45 +443,90 @@
     <t>Courier and Express</t>
   </si>
   <si>
+    <t>Long Distance Courier</t>
+  </si>
+  <si>
+    <t>3624</t>
+  </si>
+  <si>
+    <t>B2X</t>
+  </si>
+  <si>
+    <t>Premium Courier</t>
+  </si>
+  <si>
+    <t>3625</t>
+  </si>
+  <si>
+    <t>Customer setup (in FINLAND)</t>
+  </si>
+  <si>
+    <t>Standard Courier</t>
+  </si>
+  <si>
+    <t>3627</t>
+  </si>
+  <si>
+    <t>Economy Courier</t>
+  </si>
+  <si>
+    <t>3629</t>
+  </si>
+  <si>
+    <t>Long Distance Courier Truck</t>
+  </si>
+  <si>
+    <t>3654</t>
+  </si>
+  <si>
+    <t>Premium Courier Truck</t>
+  </si>
+  <si>
+    <t>3655</t>
+  </si>
+  <si>
+    <t>Standard Courier Truck</t>
+  </si>
+  <si>
+    <t>3657</t>
+  </si>
+  <si>
+    <t>Economy Courier Truck</t>
+  </si>
+  <si>
+    <t>3659</t>
+  </si>
+  <si>
+    <t>Premium Courier Bicycle</t>
+  </si>
+  <si>
+    <t>3665</t>
+  </si>
+  <si>
+    <t>Standard Courier Bicycle</t>
+  </si>
+  <si>
+    <t>3667</t>
+  </si>
+  <si>
+    <t>Economy Courier Bicycle</t>
+  </si>
+  <si>
+    <t>3669</t>
+  </si>
+  <si>
     <t>Courier Distribution</t>
   </si>
   <si>
     <t>3270</t>
   </si>
   <si>
-    <t>B2X</t>
-  </si>
-  <si>
     <t>Courier Distribution Pallet</t>
   </si>
   <si>
     <t>3271</t>
   </si>
   <si>
-    <t>Long Distance Courier</t>
-  </si>
-  <si>
-    <t>3624</t>
-  </si>
-  <si>
-    <t>Premium Courier</t>
-  </si>
-  <si>
-    <t>3625</t>
-  </si>
-  <si>
-    <t>Standard Courier</t>
-  </si>
-  <si>
-    <t>3627</t>
-  </si>
-  <si>
-    <t>Economy Courier</t>
-  </si>
-  <si>
-    <t>3629</t>
-  </si>
-  <si>
     <t>Same day distribution temp</t>
   </si>
   <si>
@@ -498,48 +543,6 @@
   </si>
   <si>
     <t>3621</t>
-  </si>
-  <si>
-    <t>Long Distance Courier Truck</t>
-  </si>
-  <si>
-    <t>3654</t>
-  </si>
-  <si>
-    <t>Premium Courier Truck</t>
-  </si>
-  <si>
-    <t>3655</t>
-  </si>
-  <si>
-    <t>Standard Courier Truck</t>
-  </si>
-  <si>
-    <t>3657</t>
-  </si>
-  <si>
-    <t>Economy Courier Truck</t>
-  </si>
-  <si>
-    <t>3659</t>
-  </si>
-  <si>
-    <t>Premium Courier Bicycle</t>
-  </si>
-  <si>
-    <t>3665</t>
-  </si>
-  <si>
-    <t>Standard Courier Bicycle</t>
-  </si>
-  <si>
-    <t>3667</t>
-  </si>
-  <si>
-    <t>Economy Courier Bicycle</t>
-  </si>
-  <si>
-    <t>3669</t>
   </si>
   <si>
     <t>Cargo Norway international</t>
@@ -767,7 +770,7 @@
     <col min="6" max="6" width="10.62109375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="7.859375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="8.265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="15.1875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="27.15625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="14.5546875" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="9.27734375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="15.76953125" customWidth="true" bestFit="true"/>
@@ -2923,7 +2926,7 @@
         <v>23</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>23</v>
@@ -2976,7 +2979,7 @@
         <v>23</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>22</v>
+        <v>147</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>23</v>
@@ -3011,13 +3014,13 @@
         <v>25</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>144</v>
@@ -3029,7 +3032,7 @@
         <v>23</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>22</v>
+        <v>147</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>23</v>
@@ -3064,13 +3067,13 @@
         <v>25</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>144</v>
@@ -3082,7 +3085,7 @@
         <v>23</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>22</v>
+        <v>147</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>23</v>
@@ -3117,13 +3120,13 @@
         <v>25</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>144</v>
@@ -3135,7 +3138,7 @@
         <v>23</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>23</v>
@@ -3170,13 +3173,13 @@
         <v>25</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>144</v>
@@ -3188,7 +3191,7 @@
         <v>23</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>23</v>
@@ -3223,16 +3226,16 @@
         <v>25</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>21</v>
+        <v>144</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>22</v>
@@ -3241,7 +3244,7 @@
         <v>23</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>23</v>
@@ -3276,13 +3279,13 @@
         <v>25</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>144</v>
@@ -3294,7 +3297,7 @@
         <v>23</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>23</v>
@@ -3329,13 +3332,13 @@
         <v>25</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>144</v>
@@ -3347,7 +3350,7 @@
         <v>23</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>23</v>
@@ -3371,7 +3374,7 @@
         <v>22</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50">
@@ -3382,13 +3385,13 @@
         <v>25</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>144</v>
@@ -3400,7 +3403,7 @@
         <v>23</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>23</v>
@@ -3424,7 +3427,7 @@
         <v>22</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51">
@@ -3435,13 +3438,13 @@
         <v>25</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>144</v>
@@ -3453,7 +3456,7 @@
         <v>23</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>23</v>
@@ -3477,7 +3480,7 @@
         <v>22</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52">
@@ -3488,13 +3491,13 @@
         <v>25</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>144</v>
@@ -3506,7 +3509,7 @@
         <v>23</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>23</v>
@@ -3541,13 +3544,13 @@
         <v>25</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>144</v>
@@ -3559,7 +3562,7 @@
         <v>23</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>23</v>
@@ -3594,16 +3597,16 @@
         <v>25</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>144</v>
+        <v>21</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>22</v>
@@ -3612,7 +3615,7 @@
         <v>23</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>23</v>
@@ -3636,7 +3639,7 @@
         <v>22</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55">
@@ -3647,13 +3650,13 @@
         <v>25</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>144</v>
@@ -3665,7 +3668,7 @@
         <v>23</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>23</v>
@@ -3689,7 +3692,7 @@
         <v>22</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56">
@@ -3700,13 +3703,13 @@
         <v>25</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>144</v>
@@ -3718,7 +3721,7 @@
         <v>23</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>23</v>
@@ -3742,24 +3745,24 @@
         <v>22</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>34</v>
@@ -3789,10 +3792,10 @@
         <v>22</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="P57" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="Q57" s="1" t="s">
         <v>22</v>
@@ -3800,19 +3803,19 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>34</v>
@@ -3859,13 +3862,13 @@
         <v>25</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>34</v>
@@ -3906,19 +3909,19 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>144</v>
@@ -3965,16 +3968,16 @@
         <v>25</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>22</v>
@@ -4004,7 +4007,7 @@
         <v>24</v>
       </c>
       <c r="P61" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="Q61" s="1" t="s">
         <v>22</v>
@@ -4012,22 +4015,22 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="1">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="1">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hide 9650 as a service from service portfolio on devsite
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -1,21 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a2344567/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83260E3-459A-C343-8BA3-159C8FB6BF68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Booking &amp; SG API" r:id="rId3" sheetId="1"/>
+    <sheet name="Booking &amp; SG API" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Booking &amp; SG API'!$A$1:$P$65</definedName>
   </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="196">
   <si>
     <t>Service family</t>
   </si>
@@ -141,12 +149,6 @@
   </si>
   <si>
     <t>9350</t>
-  </si>
-  <si>
-    <t>Return mailbox parcel</t>
-  </si>
-  <si>
-    <t>9650</t>
   </si>
   <si>
     <t>Return business parcel</t>
@@ -614,20 +616,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
       <name val="Calibri"/>
-      <sz val="12.0"/>
-      <b val="true"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -635,96 +637,16 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
-    </border>
-    <border>
-      <left>
-        <color rgb="FF000000"/>
-      </left>
-    </border>
-    <border>
-      <left>
-        <color rgb="FF000000"/>
-      </left>
-      <right>
-        <color rgb="FF000000"/>
-      </right>
-    </border>
-    <border>
-      <left>
-        <color rgb="FF000000"/>
-      </left>
-      <right>
-        <color rgb="FF000000"/>
-      </right>
-      <top>
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left>
-        <color rgb="FF000000"/>
-      </left>
-      <right>
-        <color rgb="FF000000"/>
-      </right>
-      <top>
-        <color rgb="FF000000"/>
-      </top>
-      <bottom>
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right>
-        <color rgb="FF000000"/>
-      </right>
-      <top>
-        <color rgb="FF000000"/>
-      </top>
-      <bottom>
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right>
-        <color rgb="FF000000"/>
-      </right>
-      <top>
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top>
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -739,6 +661,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -746,41 +669,369 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="0E2841"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E8E8E8"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="156082"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="E97132"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="196B24"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="0F9ED5"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="A02B93"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="4EA72E"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="467886"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="96607D"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Q65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q64"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true">
-      <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57.79296875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="21.63671875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="30.23046875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.08984375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="30.46484375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="10.62109375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="7.859375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="8.265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="27.15625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="14.5546875" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="9.27734375" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="15.76953125" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="9.73828125" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="18.35546875" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="16.00390625" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="79.9140625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="57.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="79.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -833,7 +1084,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -886,7 +1137,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -939,7 +1190,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -992,7 +1243,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1045,7 +1296,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1098,7 +1349,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1151,7 +1402,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -1204,7 +1455,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -1257,7 +1508,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1274,7 +1525,7 @@
         <v>43</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>23</v>
@@ -1310,7 +1561,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -1318,16 +1569,16 @@
         <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>23</v>
@@ -1363,27 +1614,27 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>23</v>
@@ -1404,33 +1655,33 @@
         <v>23</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>21</v>
@@ -1442,34 +1693,34 @@
         <v>23</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1477,13 +1728,13 @@
         <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>21</v>
@@ -1495,87 +1746,87 @@
         <v>23</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="N14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="Q15" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1583,13 +1834,13 @@
         <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>34</v>
@@ -1601,34 +1852,34 @@
         <v>23</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>23</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -1636,13 +1887,13 @@
         <v>25</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>34</v>
@@ -1654,34 +1905,34 @@
         <v>23</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
@@ -1689,13 +1940,13 @@
         <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>34</v>
@@ -1707,34 +1958,34 @@
         <v>23</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -1742,13 +1993,13 @@
         <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>34</v>
@@ -1760,48 +2011,48 @@
         <v>23</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="Q19" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="E20" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>34</v>
@@ -1831,16 +2082,16 @@
         <v>22</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -1851,7 +2102,7 @@
         <v>85</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>86</v>
@@ -1884,16 +2135,16 @@
         <v>22</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1904,31 +2155,31 @@
         <v>87</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>23</v>
@@ -1937,16 +2188,16 @@
         <v>22</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1954,13 +2205,13 @@
         <v>25</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>39</v>
@@ -1972,7 +2223,7 @@
         <v>23</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>23</v>
@@ -1990,16 +2241,16 @@
         <v>22</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -2007,16 +2258,16 @@
         <v>25</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>23</v>
@@ -2025,7 +2276,7 @@
         <v>23</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>23</v>
@@ -2043,16 +2294,16 @@
         <v>22</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -2060,16 +2311,16 @@
         <v>25</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>23</v>
@@ -2078,7 +2329,7 @@
         <v>23</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>23</v>
@@ -2096,16 +2347,16 @@
         <v>22</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -2113,34 +2364,34 @@
         <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>101</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>23</v>
@@ -2149,33 +2400,33 @@
         <v>22</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>104</v>
+        <v>34</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>22</v>
@@ -2184,7 +2435,7 @@
         <v>23</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>23</v>
@@ -2199,24 +2450,24 @@
         <v>23</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>106</v>
+        <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>107</v>
@@ -2237,7 +2488,7 @@
         <v>23</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>23</v>
@@ -2264,7 +2515,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -2290,7 +2541,7 @@
         <v>23</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>23</v>
@@ -2305,7 +2556,7 @@
         <v>23</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>22</v>
@@ -2317,7 +2568,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -2370,7 +2621,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -2387,10 +2638,10 @@
         <v>114</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>23</v>
@@ -2423,74 +2674,74 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>25</v>
+        <v>115</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M32" s="1" t="s">
         <v>23</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>117</v>
+        <v>25</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>21</v>
@@ -2499,10 +2750,10 @@
         <v>22</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>23</v>
@@ -2520,16 +2771,16 @@
         <v>24</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
@@ -2537,13 +2788,13 @@
         <v>25</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>21</v>
@@ -2555,7 +2806,7 @@
         <v>23</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>23</v>
@@ -2573,16 +2824,16 @@
         <v>24</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>25</v>
       </c>
@@ -2590,13 +2841,13 @@
         <v>25</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>21</v>
@@ -2608,7 +2859,7 @@
         <v>23</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>23</v>
@@ -2623,19 +2874,19 @@
         <v>23</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>25</v>
       </c>
@@ -2643,10 +2894,10 @@
         <v>25</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>129</v>
@@ -2661,7 +2912,7 @@
         <v>23</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>23</v>
@@ -2679,16 +2930,16 @@
         <v>22</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>25</v>
       </c>
@@ -2702,19 +2953,19 @@
         <v>131</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>23</v>
@@ -2732,16 +2983,16 @@
         <v>22</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>25</v>
       </c>
@@ -2749,13 +3000,13 @@
         <v>25</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>39</v>
@@ -2767,7 +3018,7 @@
         <v>23</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>23</v>
@@ -2785,16 +3036,16 @@
         <v>22</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>25</v>
       </c>
@@ -2802,13 +3053,13 @@
         <v>25</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>39</v>
@@ -2820,7 +3071,7 @@
         <v>23</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>23</v>
@@ -2838,51 +3089,51 @@
         <v>22</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>25</v>
+        <v>139</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>39</v>
+        <v>142</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M40" s="1" t="s">
         <v>23</v>
@@ -2891,34 +3142,34 @@
         <v>22</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="41">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>141</v>
+        <v>25</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="G41" s="1" t="s">
         <v>22</v>
       </c>
@@ -2926,7 +3177,7 @@
         <v>23</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>105</v>
+        <v>145</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>23</v>
@@ -2950,10 +3201,10 @@
         <v>22</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>25</v>
       </c>
@@ -2961,26 +3212,26 @@
         <v>25</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I42" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="J42" s="1" t="s">
         <v>23</v>
       </c>
@@ -3003,10 +3254,10 @@
         <v>22</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="43">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
@@ -3023,7 +3274,7 @@
         <v>149</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>22</v>
@@ -3032,7 +3283,7 @@
         <v>23</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>23</v>
@@ -3056,10 +3307,10 @@
         <v>22</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>25</v>
       </c>
@@ -3076,7 +3327,7 @@
         <v>151</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>22</v>
@@ -3085,7 +3336,7 @@
         <v>23</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>147</v>
+        <v>103</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>23</v>
@@ -3109,10 +3360,10 @@
         <v>22</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>25</v>
       </c>
@@ -3129,7 +3380,7 @@
         <v>153</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>22</v>
@@ -3138,7 +3389,7 @@
         <v>23</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>23</v>
@@ -3162,10 +3413,10 @@
         <v>22</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>25</v>
       </c>
@@ -3182,7 +3433,7 @@
         <v>155</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>22</v>
@@ -3191,7 +3442,7 @@
         <v>23</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>23</v>
@@ -3215,10 +3466,10 @@
         <v>22</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="47">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -3235,7 +3486,7 @@
         <v>157</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>22</v>
@@ -3244,7 +3495,7 @@
         <v>23</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>23</v>
@@ -3268,10 +3519,10 @@
         <v>22</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="48">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>25</v>
       </c>
@@ -3288,7 +3539,7 @@
         <v>159</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>22</v>
@@ -3297,7 +3548,7 @@
         <v>23</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>23</v>
@@ -3321,10 +3572,10 @@
         <v>22</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="49">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>25</v>
       </c>
@@ -3341,7 +3592,7 @@
         <v>161</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>22</v>
@@ -3350,7 +3601,7 @@
         <v>23</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>23</v>
@@ -3374,10 +3625,10 @@
         <v>22</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="50">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>25</v>
       </c>
@@ -3394,7 +3645,7 @@
         <v>163</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>22</v>
@@ -3403,7 +3654,7 @@
         <v>23</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>23</v>
@@ -3427,10 +3678,10 @@
         <v>22</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>25</v>
       </c>
@@ -3447,7 +3698,7 @@
         <v>165</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>22</v>
@@ -3456,7 +3707,7 @@
         <v>23</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>23</v>
@@ -3480,10 +3731,10 @@
         <v>22</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>25</v>
       </c>
@@ -3500,7 +3751,7 @@
         <v>167</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>22</v>
@@ -3509,7 +3760,7 @@
         <v>23</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>23</v>
@@ -3533,10 +3784,10 @@
         <v>22</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>25</v>
       </c>
@@ -3553,7 +3804,7 @@
         <v>169</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>144</v>
+        <v>21</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>22</v>
@@ -3562,7 +3813,7 @@
         <v>23</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>23</v>
@@ -3586,10 +3837,10 @@
         <v>22</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="54">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>25</v>
       </c>
@@ -3606,7 +3857,7 @@
         <v>171</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>21</v>
+        <v>142</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>22</v>
@@ -3615,7 +3866,7 @@
         <v>23</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>23</v>
@@ -3639,10 +3890,10 @@
         <v>22</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="55">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>25</v>
       </c>
@@ -3659,7 +3910,7 @@
         <v>173</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>22</v>
@@ -3668,7 +3919,7 @@
         <v>23</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>23</v>
@@ -3692,27 +3943,27 @@
         <v>22</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>25</v>
+        <v>174</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>144</v>
+        <v>34</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>22</v>
@@ -3721,7 +3972,7 @@
         <v>23</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>23</v>
@@ -3733,36 +3984,36 @@
         <v>23</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N56" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>22</v>
+        <v>178</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>22</v>
+        <v>178</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="E57" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>34</v>
@@ -3780,39 +4031,39 @@
         <v>23</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N57" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>180</v>
+        <v>22</v>
       </c>
       <c r="P57" s="1" t="s">
-        <v>180</v>
+        <v>22</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="58">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>181</v>
+        <v>25</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>182</v>
+        <v>25</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>182</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>183</v>
@@ -3827,7 +4078,7 @@
         <v>23</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>23</v>
@@ -3845,92 +4096,92 @@
         <v>22</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="P58" s="1" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="Q58" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q59" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="J59" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M59" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O59" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="P59" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q59" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="60">
+    <row r="60" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>186</v>
+        <v>25</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>189</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>144</v>
+        <v>190</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>22</v>
@@ -3945,96 +4196,49 @@
         <v>22</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N60" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="P60" s="1" t="s">
-        <v>22</v>
+        <v>191</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="F61" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>192</v>
       </c>
-      <c r="G61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J61" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K61" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O61" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P61" s="1" t="s">
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>193</v>
       </c>
-      <c r="Q61" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s" s="0">
+    </row>
+    <row r="63" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" t="s" s="0">
+    <row r="64" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" t="s" s="1">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s" s="1">
-        <v>197</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:P66"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <autoFilter ref="A1:P65" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{644fb37b-915b-49e6-8af0-243b8ee4c503}" enabled="1" method="Standard" siteId="{a1ae5425-0bde-496e-8c5a-8a06b0d94277}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Add 1395 VAS to service portfolio
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="197">
   <si>
     <t>Service family</t>
   </si>
@@ -182,7 +182,7 @@
     <t>NO, SE, DK, FI</t>
   </si>
   <si>
-    <t>ALL COUNTRIES EXCEPT RUSSIA, BELARUS, IRAN and ISRAEL</t>
+    <t>ALL COUNTRIES EXCEPT RUSSIA and BELARUS</t>
   </si>
   <si>
     <t>PickUp Parcel Bulk</t>
@@ -458,9 +458,6 @@
     <t>3625</t>
   </si>
   <si>
-    <t>Customer setup (in FINLAND)</t>
-  </si>
-  <si>
     <t>Standard Courier</t>
   </si>
   <si>
@@ -596,7 +593,7 @@
     <t>B2X_L</t>
   </si>
   <si>
-    <t>SE, DK, FI, AD, AE, AG, AI, AL, AM, AN, AO, AQ, AR, AS, AT, AU, AW, AX, AZ, BA, BB, BD, BE, BF, BG, BH, BI, BJ, BL, BM, BN, BO, BQ, BR, BS, BV, BW, BY, BZ, CA, CC, CD, CF, CG, CH, CI, CK, CL, CM, CN, CO, CR, CU, CV, CW, CX, CY, CZ, DE, DJ, DM, DO, DZ, EC, EE, EG, EH, ER, ES, ET, FJ, FK, FM, FO, FR, GA, GB, GD, GE, GF, GG, GH, GI, GL, GM, GN, GP, GQ, GR, GS, GT, GU, GW, GY, HK, HM, HN, HR, HT, HU, ID, IE, IM, IN, IO, IQ, IS, IT, JE, JM, JO, JP, KE, KG, KH, KI, KM, KN, KP, KR, KW, KY, KZ, LA, LB, LC, LI, LK, LR, LS, LT, LU, LV, MA, MC, MD, ME, MF, MG, MH, MK, ML, MM, MN, MO, MP, MQ, MR, MS, MT, MU, MV, MW, MX, MY, MZ, NA, NC, NE, NF, NG, NI, NL, NP, NR, NU, NZ, OM, PA, PE, PF, PG, PH, PK, PL, PM, PN, PS, PT, PW, PY, QA, RE, RO, RS, RU, RW, SA, SB, SC, SG, SH, SI, SJ, SK, SL, SM, SN, SO, SR, ST, SV, SX, SZ, TC, TD, TF, TG, TH, TJ, TK, TL, TM, TN, TO, TR, TT, TV, TW, TZ, UA, UG, UM, UY, UZ, VA, VC, VE, VG, VI, VN, VU, WF, WS, XK, YT, ZA, ZM, ZW</t>
+    <t>ALL COUNTRIES EXCEPT(NO, AF, BT, LY, SS, SD, SY, YE)</t>
   </si>
   <si>
     <t>* Only supported in Shipping Guide API</t>
@@ -770,14 +767,14 @@
     <col min="6" max="6" width="10.62109375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="7.859375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="8.265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="27.15625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="15.1875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="14.5546875" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="9.27734375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="15.76953125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="9.73828125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="18.35546875" customWidth="true" bestFit="true"/>
     <col min="15" max="15" width="16.00390625" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="255.0" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="79.9140625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2205,7 +2202,7 @@
         <v>53</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="Q27" s="1" t="s">
         <v>53</v>
@@ -2979,7 +2976,7 @@
         <v>23</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>147</v>
+        <v>105</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>23</v>
@@ -3014,13 +3011,13 @@
         <v>25</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="E43" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>144</v>
@@ -3032,7 +3029,7 @@
         <v>23</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>147</v>
+        <v>105</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>23</v>
@@ -3067,13 +3064,13 @@
         <v>25</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="E44" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>144</v>
@@ -3085,7 +3082,7 @@
         <v>23</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>147</v>
+        <v>105</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>23</v>
@@ -3120,13 +3117,13 @@
         <v>25</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="E45" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>144</v>
@@ -3173,13 +3170,13 @@
         <v>25</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="E46" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>144</v>
@@ -3226,13 +3223,13 @@
         <v>25</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="E47" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>144</v>
@@ -3279,13 +3276,13 @@
         <v>25</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="E48" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>144</v>
@@ -3332,13 +3329,13 @@
         <v>25</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="E49" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>144</v>
@@ -3385,13 +3382,13 @@
         <v>25</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="E50" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>144</v>
@@ -3438,13 +3435,13 @@
         <v>25</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="E51" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>144</v>
@@ -3491,13 +3488,13 @@
         <v>25</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="E52" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>144</v>
@@ -3544,13 +3541,13 @@
         <v>25</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="E53" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>144</v>
@@ -3597,13 +3594,13 @@
         <v>25</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="E54" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>21</v>
@@ -3650,13 +3647,13 @@
         <v>25</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="E55" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>144</v>
@@ -3703,13 +3700,13 @@
         <v>25</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="E56" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>144</v>
@@ -3750,19 +3747,19 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>34</v>
@@ -3792,10 +3789,10 @@
         <v>22</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P57" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q57" s="1" t="s">
         <v>22</v>
@@ -3803,19 +3800,19 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>34</v>
@@ -3862,13 +3859,13 @@
         <v>25</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>34</v>
@@ -3909,19 +3906,19 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C60" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>144</v>
@@ -3968,16 +3965,16 @@
         <v>25</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="E61" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>22</v>
@@ -4007,7 +4004,7 @@
         <v>24</v>
       </c>
       <c r="P61" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q61" s="1" t="s">
         <v>22</v>
@@ -4015,22 +4012,22 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="1">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="1">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replacing CARGO_INTERNATIONAL with 4000
</commit_message>
<xml_diff>
--- a/static/services/services_booking_shippingguide.xlsx
+++ b/static/services/services_booking_shippingguide.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Booking &amp; SG API" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Booking &amp; SG API'!$A$1:$P$65</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="195">
   <si>
     <t>Service family</t>
   </si>
@@ -143,12 +143,6 @@
     <t>9350</t>
   </si>
   <si>
-    <t>Return mailbox parcel</t>
-  </si>
-  <si>
-    <t>9650</t>
-  </si>
-  <si>
     <t>Return business parcel</t>
   </si>
   <si>
@@ -548,19 +542,19 @@
     <t>Cargo International</t>
   </si>
   <si>
+    <t>4000</t>
+  </si>
+  <si>
+    <t>NO, Europe</t>
+  </si>
+  <si>
+    <t>Supply base logistics</t>
+  </si>
+  <si>
+    <t>Supply Base Logistics</t>
+  </si>
+  <si>
     <t>3050</t>
-  </si>
-  <si>
-    <t>CARGO_INTERNATIONAL</t>
-  </si>
-  <si>
-    <t>NO, Europe**</t>
-  </si>
-  <si>
-    <t>Supply base logistics</t>
-  </si>
-  <si>
-    <t>Supply Base Logistics</t>
   </si>
   <si>
     <t>OIL_EXPRESS</t>
@@ -750,7 +744,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Q65"/>
+  <dimension ref="A1:Q64"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -1271,7 +1265,7 @@
         <v>43</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>23</v>
@@ -1315,16 +1309,16 @@
         <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>23</v>
@@ -1362,25 +1356,25 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>23</v>
@@ -1401,33 +1395,33 @@
         <v>23</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>21</v>
@@ -1439,31 +1433,31 @@
         <v>23</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14">
@@ -1474,13 +1468,13 @@
         <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>21</v>
@@ -1492,31 +1486,31 @@
         <v>23</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15">
@@ -1527,49 +1521,49 @@
         <v>25</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="O15" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16">
@@ -1580,13 +1574,13 @@
         <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>34</v>
@@ -1598,31 +1592,31 @@
         <v>23</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>23</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17">
@@ -1633,13 +1627,13 @@
         <v>25</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>34</v>
@@ -1651,31 +1645,31 @@
         <v>23</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18">
@@ -1686,13 +1680,13 @@
         <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>34</v>
@@ -1704,31 +1698,31 @@
         <v>23</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19">
@@ -1739,13 +1733,13 @@
         <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>34</v>
@@ -1757,31 +1751,31 @@
         <v>23</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20">
@@ -1792,13 +1786,13 @@
         <v>25</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>34</v>
@@ -1828,13 +1822,13 @@
         <v>22</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21">
@@ -1848,7 +1842,7 @@
         <v>85</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>86</v>
@@ -1881,13 +1875,13 @@
         <v>22</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22">
@@ -1901,31 +1895,31 @@
         <v>87</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>23</v>
@@ -1934,13 +1928,13 @@
         <v>22</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23">
@@ -1951,13 +1945,13 @@
         <v>25</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>39</v>
@@ -1969,7 +1963,7 @@
         <v>23</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>23</v>
@@ -1987,13 +1981,13 @@
         <v>22</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24">
@@ -2004,16 +1998,16 @@
         <v>25</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>23</v>
@@ -2022,7 +2016,7 @@
         <v>23</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>23</v>
@@ -2040,13 +2034,13 @@
         <v>22</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25">
@@ -2057,16 +2051,16 @@
         <v>25</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>23</v>
@@ -2075,7 +2069,7 @@
         <v>23</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>23</v>
@@ -2093,13 +2087,13 @@
         <v>22</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26">
@@ -2110,34 +2104,34 @@
         <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>101</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>23</v>
@@ -2146,33 +2140,33 @@
         <v>22</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>104</v>
+        <v>34</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>22</v>
@@ -2181,7 +2175,7 @@
         <v>23</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>23</v>
@@ -2196,24 +2190,24 @@
         <v>23</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>106</v>
+        <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>107</v>
@@ -2234,7 +2228,7 @@
         <v>23</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>23</v>
@@ -2287,7 +2281,7 @@
         <v>23</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>23</v>
@@ -2302,7 +2296,7 @@
         <v>23</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>22</v>
@@ -2384,10 +2378,10 @@
         <v>114</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>23</v>
@@ -2422,72 +2416,72 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>25</v>
+        <v>115</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M32" s="1" t="s">
         <v>23</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>117</v>
+        <v>25</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>21</v>
@@ -2496,10 +2490,10 @@
         <v>22</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>23</v>
@@ -2517,13 +2511,13 @@
         <v>24</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34">
@@ -2534,13 +2528,13 @@
         <v>25</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>21</v>
@@ -2552,7 +2546,7 @@
         <v>23</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>23</v>
@@ -2570,13 +2564,13 @@
         <v>24</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35">
@@ -2587,13 +2581,13 @@
         <v>25</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>21</v>
@@ -2605,7 +2599,7 @@
         <v>23</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>23</v>
@@ -2620,16 +2614,16 @@
         <v>23</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36">
@@ -2640,10 +2634,10 @@
         <v>25</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>129</v>
@@ -2658,7 +2652,7 @@
         <v>23</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>23</v>
@@ -2676,13 +2670,13 @@
         <v>22</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37">
@@ -2699,19 +2693,19 @@
         <v>131</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>23</v>
@@ -2729,13 +2723,13 @@
         <v>22</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38">
@@ -2746,13 +2740,13 @@
         <v>25</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>39</v>
@@ -2764,7 +2758,7 @@
         <v>23</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>23</v>
@@ -2782,13 +2776,13 @@
         <v>22</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39">
@@ -2799,13 +2793,13 @@
         <v>25</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>39</v>
@@ -2817,7 +2811,7 @@
         <v>23</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>23</v>
@@ -2835,51 +2829,51 @@
         <v>22</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>25</v>
+        <v>139</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>39</v>
+        <v>142</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M40" s="1" t="s">
         <v>23</v>
@@ -2888,34 +2882,34 @@
         <v>22</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>141</v>
+        <v>25</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="G41" s="1" t="s">
         <v>22</v>
       </c>
@@ -2923,7 +2917,7 @@
         <v>23</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>23</v>
@@ -2947,7 +2941,7 @@
         <v>22</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42">
@@ -2967,7 +2961,7 @@
         <v>146</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>22</v>
@@ -2976,7 +2970,7 @@
         <v>23</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>23</v>
@@ -3000,7 +2994,7 @@
         <v>22</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43">
@@ -3020,7 +3014,7 @@
         <v>148</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>22</v>
@@ -3029,7 +3023,7 @@
         <v>23</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>23</v>
@@ -3053,7 +3047,7 @@
         <v>22</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44">
@@ -3073,7 +3067,7 @@
         <v>150</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>22</v>
@@ -3082,7 +3076,7 @@
         <v>23</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>23</v>
@@ -3106,7 +3100,7 @@
         <v>22</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45">
@@ -3126,7 +3120,7 @@
         <v>152</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>22</v>
@@ -3135,7 +3129,7 @@
         <v>23</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>23</v>
@@ -3159,7 +3153,7 @@
         <v>22</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46">
@@ -3179,7 +3173,7 @@
         <v>154</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>22</v>
@@ -3188,7 +3182,7 @@
         <v>23</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>23</v>
@@ -3212,7 +3206,7 @@
         <v>22</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47">
@@ -3232,7 +3226,7 @@
         <v>156</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>22</v>
@@ -3241,7 +3235,7 @@
         <v>23</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>23</v>
@@ -3265,7 +3259,7 @@
         <v>22</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48">
@@ -3285,7 +3279,7 @@
         <v>158</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>22</v>
@@ -3294,7 +3288,7 @@
         <v>23</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>23</v>
@@ -3318,7 +3312,7 @@
         <v>22</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49">
@@ -3338,7 +3332,7 @@
         <v>160</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>22</v>
@@ -3347,7 +3341,7 @@
         <v>23</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>23</v>
@@ -3371,7 +3365,7 @@
         <v>22</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50">
@@ -3391,7 +3385,7 @@
         <v>162</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>22</v>
@@ -3400,7 +3394,7 @@
         <v>23</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>23</v>
@@ -3424,7 +3418,7 @@
         <v>22</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51">
@@ -3444,7 +3438,7 @@
         <v>164</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>22</v>
@@ -3453,7 +3447,7 @@
         <v>23</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>23</v>
@@ -3477,7 +3471,7 @@
         <v>22</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52">
@@ -3497,7 +3491,7 @@
         <v>166</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>22</v>
@@ -3506,7 +3500,7 @@
         <v>23</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>23</v>
@@ -3530,7 +3524,7 @@
         <v>22</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53">
@@ -3550,7 +3544,7 @@
         <v>168</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>144</v>
+        <v>21</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>22</v>
@@ -3559,7 +3553,7 @@
         <v>23</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>23</v>
@@ -3583,7 +3577,7 @@
         <v>22</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54">
@@ -3603,7 +3597,7 @@
         <v>170</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>21</v>
+        <v>142</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>22</v>
@@ -3612,7 +3606,7 @@
         <v>23</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>23</v>
@@ -3636,7 +3630,7 @@
         <v>22</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55">
@@ -3656,7 +3650,7 @@
         <v>172</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>22</v>
@@ -3665,7 +3659,7 @@
         <v>23</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>23</v>
@@ -3689,27 +3683,27 @@
         <v>22</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>25</v>
+        <v>173</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>144</v>
+        <v>34</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>22</v>
@@ -3718,7 +3712,7 @@
         <v>23</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>23</v>
@@ -3730,36 +3724,36 @@
         <v>23</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N56" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>22</v>
+        <v>176</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>22</v>
+        <v>176</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>18</v>
+        <v>178</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>34</v>
@@ -3777,39 +3771,39 @@
         <v>23</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N57" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>179</v>
+        <v>22</v>
       </c>
       <c r="P57" s="1" t="s">
-        <v>179</v>
+        <v>22</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>180</v>
+        <v>25</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>181</v>
+        <v>25</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>181</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>182</v>
@@ -3824,7 +3818,7 @@
         <v>23</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>23</v>
@@ -3842,48 +3836,48 @@
         <v>22</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="P58" s="1" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="Q58" s="1" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>25</v>
+        <v>183</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>34</v>
+        <v>142</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L59" s="1" t="s">
         <v>22</v>
@@ -3895,39 +3889,39 @@
         <v>22</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="Q59" s="1" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>185</v>
+        <v>25</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>188</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>144</v>
+        <v>189</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>22</v>
@@ -3942,96 +3936,43 @@
         <v>22</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N60" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="P60" s="1" t="s">
-        <v>22</v>
+        <v>190</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F61" s="1" t="s">
+      <c r="A61" t="s" s="0">
         <v>191</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J61" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K61" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O61" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P61" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q61" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="1">
         <v>193</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s" s="0">
-        <v>194</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="1">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s" s="1">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P66"/>
+  <autoFilter ref="A1:P65"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>